<commit_message>
Actualizacion a la evaluación en español
</commit_message>
<xml_diff>
--- a/SPREADSHEETS/Survey Form-Spanish.xlsx
+++ b/SPREADSHEETS/Survey Form-Spanish.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="565">
   <si>
     <t xml:space="preserve">1. To have experienced or been exposed to </t>
   </si>
@@ -336,51 +336,6 @@
     <t>DESIGNING</t>
   </si>
   <si>
-    <t xml:space="preserve">Considerations for human user/operators </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consideration of sustainability </t>
-  </si>
-  <si>
-    <t>The manufacturing of parts</t>
-  </si>
-  <si>
-    <t>The assembly of parts into larger constructs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tolerances, variability, key characteristics and statistical process control </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The break down of high-level components into module designs (including algorithms and data structures) </t>
-  </si>
-  <si>
-    <t>The low-level design (coding)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The system build </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The integration of software in electronic hardware (size of processor, communications, etc.) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The integration of software with sensor, actuators and mechanical hardware </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hardware/software function and safety </t>
-  </si>
-  <si>
-    <t>The validation of performance to customer needs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The certification to standards </t>
-  </si>
-  <si>
-    <t>Supply chains and logistics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Control of implementation cost, performance and schedule </t>
-  </si>
-  <si>
     <t>4.4.5</t>
   </si>
   <si>
@@ -411,132 +366,9 @@
     <t>IMPLEMENTING</t>
   </si>
   <si>
-    <t xml:space="preserve">Designing a Sustainable Implementation Process </t>
-  </si>
-  <si>
-    <t>The goals and metrics for implementation performance, cost and quality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The implementation system design: </t>
-  </si>
-  <si>
-    <t>Task allocation and cell/unit layout</t>
-  </si>
-  <si>
-    <t>Work flow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hardware Manufacturing Process </t>
-  </si>
-  <si>
-    <t>Algorithms (data structures, control flow, data flow)</t>
-  </si>
-  <si>
-    <t>The programming language and paradigms</t>
-  </si>
-  <si>
-    <t>Test and analysis procedures (hardware vs. software, acceptance vs. qualification)</t>
-  </si>
-  <si>
-    <t>The verification of performance to system requirements</t>
-  </si>
-  <si>
-    <t>The organization and structure for implementation</t>
-  </si>
-  <si>
     <t>Sourcing and partnering</t>
   </si>
   <si>
-    <t xml:space="preserve">Software Implementing Process </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hardware Software Integration </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test, Verification, Validation and Certification </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementation Management </t>
-  </si>
-  <si>
-    <t>Quality assurance</t>
-  </si>
-  <si>
-    <t>Human health and safety</t>
-  </si>
-  <si>
-    <t>Environmental security</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Possible implementation process improvements </t>
-  </si>
-  <si>
-    <t>The goals and metrics for operational performance, cost and value Sustainable operations</t>
-  </si>
-  <si>
-    <t>Safe and secure operations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operations process architecture and development </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operations (and mission) analysis and modeling </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instruction and programs </t>
-  </si>
-  <si>
-    <t>Procedures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operations process interactions </t>
-  </si>
-  <si>
-    <t>Maintenance and logistics</t>
-  </si>
-  <si>
-    <t>Life cycle performance and reliability</t>
-  </si>
-  <si>
-    <t>Life cycle value and costs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feedback to facilitate system improvement </t>
-  </si>
-  <si>
-    <t>Pre-planned product improvement</t>
-  </si>
-  <si>
-    <t>Improvements based on needs observed in operation</t>
-  </si>
-  <si>
-    <t>Evolutionary system upgrades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contingency improvements/solutions resulting from operational necessity </t>
-  </si>
-  <si>
-    <t>The end of useful life</t>
-  </si>
-  <si>
-    <t>Disposal options</t>
-  </si>
-  <si>
-    <t>Residual value at life-end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Environmental considerations for disposal </t>
-  </si>
-  <si>
-    <t>Possible operations process improvements</t>
-  </si>
-  <si>
-    <t>Life cycle management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Environmental security </t>
-  </si>
-  <si>
     <t>4.6.0</t>
   </si>
   <si>
@@ -561,48 +393,6 @@
     <t>OPERATING</t>
   </si>
   <si>
-    <t xml:space="preserve">Designing and Optimizing Sustainable and Safe Operations </t>
-  </si>
-  <si>
-    <t>Training for professional operations:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simulation </t>
-  </si>
-  <si>
-    <t>Education for consumer operation</t>
-  </si>
-  <si>
-    <t>Operations processes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Training and Operations </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supporting the System Life Cycle </t>
-  </si>
-  <si>
-    <t xml:space="preserve">System Improvement and Evolution </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disposal and Life-End Issues </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operations Management </t>
-  </si>
-  <si>
-    <t>The organization and structure for operations</t>
-  </si>
-  <si>
-    <t>Partnerships and alliances</t>
-  </si>
-  <si>
-    <t>Control of operations cost, performance and scheduling</t>
-  </si>
-  <si>
-    <t>Quality and safety assurance</t>
-  </si>
-  <si>
     <t>ETHICS, EQUITY AND OTHER RESPONSIBILITIES</t>
   </si>
   <si>
@@ -1714,6 +1504,219 @@
   </si>
   <si>
     <t>Retiro, reutilizacion y reciclaje</t>
+  </si>
+  <si>
+    <t>Diseñando un Proceso de Implementacion Sostenible</t>
+  </si>
+  <si>
+    <t>Los objetivos y metricas de rendimiento de la aplicacion, costo y calidad</t>
+  </si>
+  <si>
+    <t>El diseño del sistema de implementacion:</t>
+  </si>
+  <si>
+    <t>Asignacion de tareas y cell/unit layout</t>
+  </si>
+  <si>
+    <t>Flujo de trabajo</t>
+  </si>
+  <si>
+    <t>Consideraciones para los usuarios/operadores humanos</t>
+  </si>
+  <si>
+    <t>Consideraciones de sostenibilidad</t>
+  </si>
+  <si>
+    <t>Proceso de Fabricacion de Hardware</t>
+  </si>
+  <si>
+    <t>La fabricacion de piezas</t>
+  </si>
+  <si>
+    <t>El montaje de piezas en construcciones mayores</t>
+  </si>
+  <si>
+    <t>Control de tolerancia, variabilidad, caracteristicas claves y procesos estadisticos</t>
+  </si>
+  <si>
+    <t>Proceso de Implementacion de Software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El desgloce de componentes de alto nivel en modulos de diseño (incluyendo algoritmos y estructuras de datos) </t>
+  </si>
+  <si>
+    <t>Algoritmos (estructuras de datos, control de flujo, flujo de datos)</t>
+  </si>
+  <si>
+    <t>El lenguaje y paradigmas de programacion</t>
+  </si>
+  <si>
+    <t>El diseño de bajo nivel (codigo)</t>
+  </si>
+  <si>
+    <t>La construccion del sistema</t>
+  </si>
+  <si>
+    <t>Integracion de Hardware y Software</t>
+  </si>
+  <si>
+    <t>La integracion del software con sensores, controladores y hardware mecanico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La integracion del software con hardware electronico (capacidad del procesador, comunicaciones, etc.) </t>
+  </si>
+  <si>
+    <t>Funcionamiento y seguridad del Hardware/Software</t>
+  </si>
+  <si>
+    <t>Pruebas, Verificacion, Validacion y Certificacion</t>
+  </si>
+  <si>
+    <t>Procedimientos de pruebas y analisis (hardware vs. software, aceptacion vs. Calificacion)</t>
+  </si>
+  <si>
+    <t>La verifiacion del rendimiento a los requerimientos del sistema</t>
+  </si>
+  <si>
+    <t>La validacion del rendimiento con las necesidades de los clientes</t>
+  </si>
+  <si>
+    <t>La cerificacion de estandares</t>
+  </si>
+  <si>
+    <t>Gestion de la Implementacion</t>
+  </si>
+  <si>
+    <t>La organizacion y estructura para la implementacion</t>
+  </si>
+  <si>
+    <t>Cadenas de suministro y logistica</t>
+  </si>
+  <si>
+    <t>Control de los costos, rendimiento y cronograma de la implementacion</t>
+  </si>
+  <si>
+    <t>Aseguramiento de la calidad</t>
+  </si>
+  <si>
+    <t>Salud y seguridad humana</t>
+  </si>
+  <si>
+    <t>Seguridad ambiental</t>
+  </si>
+  <si>
+    <t>Posibles mejoras al proceso de implementacion</t>
+  </si>
+  <si>
+    <t>Diseñar y Optimizar Operaciones Sostenibles y Seguras</t>
+  </si>
+  <si>
+    <t>Los objetivos y metricas para el rendimiento operacional, valor y costos de operaciones sostenibles</t>
+  </si>
+  <si>
+    <t>Operaciones seguras y protegidas</t>
+  </si>
+  <si>
+    <t>Arquitectura y desarrollo del proceso de operaciones</t>
+  </si>
+  <si>
+    <t>Analisis y modelado de las operaciones (y de la mision)</t>
+  </si>
+  <si>
+    <t>Entrenamiento y Operaciones</t>
+  </si>
+  <si>
+    <t>Entrenar para operaciones profesionales:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SImulacion </t>
+  </si>
+  <si>
+    <t>Instrucción y programas</t>
+  </si>
+  <si>
+    <t>Procedimientos</t>
+  </si>
+  <si>
+    <t>Educacion para la operacion de los consumidores</t>
+  </si>
+  <si>
+    <t>Procesos de operaciones</t>
+  </si>
+  <si>
+    <t>Interaccion entre procesos de operaciones</t>
+  </si>
+  <si>
+    <t>Apoyar el Ciclo de Vida del Sistema</t>
+  </si>
+  <si>
+    <t>Mantenimiento y logistica</t>
+  </si>
+  <si>
+    <t>Rendimiento y confiabilidad del ciclo de vida</t>
+  </si>
+  <si>
+    <t>Valor y costos del ciclo de vida</t>
+  </si>
+  <si>
+    <t>Retroalimentacion para facilitar la mejora del sistema</t>
+  </si>
+  <si>
+    <t>Mejora y Evolucion del Sistema</t>
+  </si>
+  <si>
+    <t>Mejoras pre-planeadas para el producto</t>
+  </si>
+  <si>
+    <t>Mejoras con base en las necesidades detectadas en el funcionamiento</t>
+  </si>
+  <si>
+    <t>Actualizaciones evolutivas del sistema</t>
+  </si>
+  <si>
+    <t>Soluciones/Mejoras de contingencia resultantes de la necesidad operacional</t>
+  </si>
+  <si>
+    <t>Cuestiones relativas a la Eliminacion y Life-End (Disposal and Life-End Issues)</t>
+  </si>
+  <si>
+    <t>La terminacion de la vida util</t>
+  </si>
+  <si>
+    <t>Opciones de eliminacion</t>
+  </si>
+  <si>
+    <t>Valor residual al life-end</t>
+  </si>
+  <si>
+    <t>Consideraciones ambientales para la eliminacion</t>
+  </si>
+  <si>
+    <t>Gestion de Operaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La organización y la estructura para las operaciones </t>
+  </si>
+  <si>
+    <t>Asociaciones y alianzas</t>
+  </si>
+  <si>
+    <t>Control de costos, desempeño y programacion de operaciones</t>
+  </si>
+  <si>
+    <t>Aseguramiento de la calidad y la seguridad</t>
+  </si>
+  <si>
+    <t>Posibles mejoras al proceso operacional</t>
+  </si>
+  <si>
+    <t>Gestion del ciclo de vida</t>
+  </si>
+  <si>
+    <t>Salud y Seguridad Humana</t>
+  </si>
+  <si>
+    <t>Seguridad Ambiental</t>
   </si>
 </sst>
 </file>
@@ -1777,7 +1780,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1810,6 +1813,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1880,7 +1889,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1903,6 +1912,8 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Buena 2" xfId="6"/>
@@ -2260,8 +2271,8 @@
   </sheetPr>
   <dimension ref="A1:G557"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A471" workbookViewId="0">
-      <selection activeCell="C480" sqref="C480"/>
+    <sheetView tabSelected="1" topLeftCell="A532" workbookViewId="0">
+      <selection activeCell="C557" sqref="C557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="3" x14ac:dyDescent="0"/>
@@ -2318,7 +2329,7 @@
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="12" t="s">
-        <v>227</v>
+        <v>157</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>0</v>
@@ -2328,7 +2339,7 @@
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9" t="s">
-        <v>194</v>
+        <v>124</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>1</v>
@@ -2338,7 +2349,7 @@
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
-        <v>195</v>
+        <v>125</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>2</v>
@@ -2348,7 +2359,7 @@
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9" t="s">
-        <v>196</v>
+        <v>126</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>3</v>
@@ -2358,7 +2369,7 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
-        <v>197</v>
+        <v>127</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>4</v>
@@ -2375,21 +2386,21 @@
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="12" t="s">
-        <v>198</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:7" outlineLevel="3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9" t="s">
-        <v>199</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:7" outlineLevel="3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9" t="s">
-        <v>200</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:7" outlineLevel="2">
@@ -2403,21 +2414,21 @@
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="12" t="s">
-        <v>228</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:3" outlineLevel="3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9" t="s">
-        <v>201</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:3" outlineLevel="3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9" t="s">
-        <v>202</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:3" outlineLevel="2">
@@ -2431,35 +2442,35 @@
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="12" t="s">
-        <v>229</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:3" outlineLevel="3">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9" t="s">
-        <v>203</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:3" outlineLevel="3">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="9" t="s">
-        <v>204</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:3" outlineLevel="3">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="9" t="s">
-        <v>205</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:3" outlineLevel="3">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9" t="s">
-        <v>206</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:3" outlineLevel="2">
@@ -2473,35 +2484,35 @@
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="12" t="s">
-        <v>230</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:3" outlineLevel="3">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9" t="s">
-        <v>207</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:3" outlineLevel="3">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9" t="s">
-        <v>208</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:3" outlineLevel="3">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9" t="s">
-        <v>209</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:3" outlineLevel="3">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="9" t="s">
-        <v>210</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:3" outlineLevel="1">
@@ -2529,21 +2540,21 @@
       </c>
       <c r="B34" s="13"/>
       <c r="C34" s="12" t="s">
-        <v>231</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:3" outlineLevel="3">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="9" t="s">
-        <v>211</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:3" outlineLevel="3">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="9" t="s">
-        <v>212</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:3" outlineLevel="2">
@@ -2557,49 +2568,49 @@
       </c>
       <c r="B38" s="13"/>
       <c r="C38" s="12" t="s">
-        <v>232</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:3" outlineLevel="3">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="9" t="s">
-        <v>213</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:3" outlineLevel="3">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="9" t="s">
-        <v>214</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:3" outlineLevel="3">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="9" t="s">
-        <v>215</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:3" outlineLevel="3">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="15" t="s">
-        <v>216</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:3" outlineLevel="3">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="9" t="s">
-        <v>217</v>
+        <v>147</v>
       </c>
     </row>
     <row r="44" spans="1:3" outlineLevel="3">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="9" t="s">
-        <v>218</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:3" outlineLevel="2">
@@ -2613,42 +2624,42 @@
       </c>
       <c r="B46" s="13"/>
       <c r="C46" s="12" t="s">
-        <v>233</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:3" outlineLevel="3">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="9" t="s">
-        <v>219</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:3" outlineLevel="3">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="9" t="s">
-        <v>220</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:3" outlineLevel="3">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="9" t="s">
-        <v>221</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:3" outlineLevel="3">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="9" t="s">
-        <v>222</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:3" outlineLevel="3">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="9" t="s">
-        <v>223</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:3" outlineLevel="2">
@@ -2662,28 +2673,28 @@
       </c>
       <c r="B53" s="13"/>
       <c r="C53" s="12" t="s">
-        <v>234</v>
+        <v>164</v>
       </c>
     </row>
     <row r="54" spans="1:3" outlineLevel="3">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="9" t="s">
-        <v>224</v>
+        <v>154</v>
       </c>
     </row>
     <row r="55" spans="1:3" outlineLevel="3">
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="9" t="s">
-        <v>225</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:3" outlineLevel="3">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="9" t="s">
-        <v>226</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:3" outlineLevel="1">
@@ -2711,35 +2722,35 @@
       </c>
       <c r="B60" s="13"/>
       <c r="C60" s="12" t="s">
-        <v>235</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:3" outlineLevel="3">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="9" t="s">
-        <v>236</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:3" outlineLevel="3">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="9" t="s">
-        <v>237</v>
+        <v>167</v>
       </c>
     </row>
     <row r="63" spans="1:3" outlineLevel="3">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="9" t="s">
-        <v>238</v>
+        <v>168</v>
       </c>
     </row>
     <row r="64" spans="1:3" outlineLevel="3">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="9" t="s">
-        <v>239</v>
+        <v>169</v>
       </c>
     </row>
     <row r="65" spans="1:3" outlineLevel="2">
@@ -2753,35 +2764,35 @@
       </c>
       <c r="B66" s="13"/>
       <c r="C66" s="12" t="s">
-        <v>240</v>
+        <v>170</v>
       </c>
     </row>
     <row r="67" spans="1:3" outlineLevel="3">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="9" t="s">
-        <v>241</v>
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:3" outlineLevel="3">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="9" t="s">
-        <v>242</v>
+        <v>172</v>
       </c>
     </row>
     <row r="69" spans="1:3" outlineLevel="3">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="9" t="s">
-        <v>243</v>
+        <v>173</v>
       </c>
     </row>
     <row r="70" spans="1:3" outlineLevel="3">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="9" t="s">
-        <v>244</v>
+        <v>174</v>
       </c>
     </row>
     <row r="71" spans="1:3" outlineLevel="2">
@@ -2795,28 +2806,28 @@
       </c>
       <c r="B72" s="13"/>
       <c r="C72" s="12" t="s">
-        <v>245</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:3" outlineLevel="3">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="9" t="s">
-        <v>246</v>
+        <v>176</v>
       </c>
     </row>
     <row r="74" spans="1:3" outlineLevel="3">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="9" t="s">
-        <v>248</v>
+        <v>178</v>
       </c>
     </row>
     <row r="75" spans="1:3" outlineLevel="3">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="9" t="s">
-        <v>247</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:3" outlineLevel="2">
@@ -2830,28 +2841,28 @@
       </c>
       <c r="B77" s="13"/>
       <c r="C77" s="12" t="s">
-        <v>249</v>
+        <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:3" outlineLevel="3">
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="9" t="s">
-        <v>250</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="1:3" outlineLevel="3">
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="C79" s="9" t="s">
-        <v>251</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:3" outlineLevel="3">
       <c r="A80" s="8"/>
       <c r="B80" s="8"/>
       <c r="C80" s="9" t="s">
-        <v>252</v>
+        <v>182</v>
       </c>
     </row>
     <row r="81" spans="1:3" outlineLevel="1">
@@ -2879,35 +2890,35 @@
       </c>
       <c r="B84" s="13"/>
       <c r="C84" s="12" t="s">
-        <v>253</v>
+        <v>183</v>
       </c>
     </row>
     <row r="85" spans="1:3" outlineLevel="3">
       <c r="A85" s="8"/>
       <c r="B85" s="8"/>
       <c r="C85" s="9" t="s">
-        <v>254</v>
+        <v>184</v>
       </c>
     </row>
     <row r="86" spans="1:3" outlineLevel="3">
       <c r="A86" s="8"/>
       <c r="B86" s="8"/>
       <c r="C86" s="9" t="s">
-        <v>255</v>
+        <v>185</v>
       </c>
     </row>
     <row r="87" spans="1:3" outlineLevel="3">
       <c r="A87" s="8"/>
       <c r="B87" s="8"/>
       <c r="C87" s="9" t="s">
-        <v>256</v>
+        <v>186</v>
       </c>
     </row>
     <row r="88" spans="1:3" outlineLevel="3">
       <c r="A88" s="8"/>
       <c r="B88" s="8"/>
       <c r="C88" s="9" t="s">
-        <v>257</v>
+        <v>187</v>
       </c>
     </row>
     <row r="89" spans="1:3" outlineLevel="2">
@@ -2921,70 +2932,70 @@
       </c>
       <c r="B90" s="13"/>
       <c r="C90" s="12" t="s">
-        <v>258</v>
+        <v>188</v>
       </c>
     </row>
     <row r="91" spans="1:3" outlineLevel="3">
       <c r="A91" s="8"/>
       <c r="B91" s="8"/>
       <c r="C91" s="9" t="s">
-        <v>259</v>
+        <v>189</v>
       </c>
     </row>
     <row r="92" spans="1:3" outlineLevel="3">
       <c r="A92" s="8"/>
       <c r="B92" s="8"/>
       <c r="C92" s="9" t="s">
-        <v>260</v>
+        <v>190</v>
       </c>
     </row>
     <row r="93" spans="1:3" outlineLevel="3">
       <c r="A93" s="8"/>
       <c r="B93" s="8"/>
       <c r="C93" s="9" t="s">
-        <v>261</v>
+        <v>191</v>
       </c>
     </row>
     <row r="94" spans="1:3" outlineLevel="3">
       <c r="A94" s="8"/>
       <c r="B94" s="8"/>
       <c r="C94" s="9" t="s">
-        <v>262</v>
+        <v>192</v>
       </c>
     </row>
     <row r="95" spans="1:3" outlineLevel="3">
       <c r="A95" s="8"/>
       <c r="B95" s="8"/>
       <c r="C95" s="9" t="s">
-        <v>263</v>
+        <v>193</v>
       </c>
     </row>
     <row r="96" spans="1:3" outlineLevel="3">
       <c r="A96" s="8"/>
       <c r="B96" s="8"/>
       <c r="C96" s="9" t="s">
-        <v>264</v>
+        <v>194</v>
       </c>
     </row>
     <row r="97" spans="1:3" outlineLevel="3">
       <c r="A97" s="8"/>
       <c r="B97" s="8"/>
       <c r="C97" s="9" t="s">
-        <v>265</v>
+        <v>195</v>
       </c>
     </row>
     <row r="98" spans="1:3" outlineLevel="3">
       <c r="A98" s="8"/>
       <c r="B98" s="8"/>
       <c r="C98" s="9" t="s">
-        <v>266</v>
+        <v>196</v>
       </c>
     </row>
     <row r="99" spans="1:3" outlineLevel="3">
       <c r="A99" s="8"/>
       <c r="B99" s="8"/>
       <c r="C99" s="9" t="s">
-        <v>267</v>
+        <v>197</v>
       </c>
     </row>
     <row r="100" spans="1:3" outlineLevel="2">
@@ -2998,35 +3009,35 @@
       </c>
       <c r="B101" s="13"/>
       <c r="C101" s="12" t="s">
-        <v>268</v>
+        <v>198</v>
       </c>
     </row>
     <row r="102" spans="1:3" outlineLevel="3">
       <c r="A102" s="8"/>
       <c r="B102" s="8"/>
       <c r="C102" s="9" t="s">
-        <v>269</v>
+        <v>199</v>
       </c>
     </row>
     <row r="103" spans="1:3" outlineLevel="3">
       <c r="A103" s="8"/>
       <c r="B103" s="8"/>
       <c r="C103" s="9" t="s">
-        <v>270</v>
+        <v>200</v>
       </c>
     </row>
     <row r="104" spans="1:3" outlineLevel="3">
       <c r="A104" s="8"/>
       <c r="B104" s="8"/>
       <c r="C104" s="9" t="s">
-        <v>271</v>
+        <v>201</v>
       </c>
     </row>
     <row r="105" spans="1:3" outlineLevel="3">
       <c r="A105" s="8"/>
       <c r="B105" s="8"/>
       <c r="C105" s="9" t="s">
-        <v>272</v>
+        <v>202</v>
       </c>
     </row>
     <row r="106" spans="1:3" outlineLevel="2">
@@ -3040,49 +3051,49 @@
       </c>
       <c r="B107" s="13"/>
       <c r="C107" s="12" t="s">
-        <v>273</v>
+        <v>203</v>
       </c>
     </row>
     <row r="108" spans="1:3" outlineLevel="3">
       <c r="A108" s="8"/>
       <c r="B108" s="8"/>
       <c r="C108" s="9" t="s">
-        <v>274</v>
+        <v>204</v>
       </c>
     </row>
     <row r="109" spans="1:3" outlineLevel="3">
       <c r="A109" s="8"/>
       <c r="B109" s="8"/>
       <c r="C109" s="9" t="s">
-        <v>275</v>
+        <v>205</v>
       </c>
     </row>
     <row r="110" spans="1:3" outlineLevel="3">
       <c r="A110" s="8"/>
       <c r="B110" s="8"/>
       <c r="C110" s="9" t="s">
-        <v>276</v>
+        <v>206</v>
       </c>
     </row>
     <row r="111" spans="1:3" outlineLevel="3">
       <c r="A111" s="8"/>
       <c r="B111" s="8"/>
       <c r="C111" s="9" t="s">
-        <v>277</v>
+        <v>207</v>
       </c>
     </row>
     <row r="112" spans="1:3" outlineLevel="3">
       <c r="A112" s="8"/>
       <c r="B112" s="8"/>
       <c r="C112" s="9" t="s">
-        <v>278</v>
+        <v>208</v>
       </c>
     </row>
     <row r="113" spans="1:3" outlineLevel="3">
       <c r="A113" s="8"/>
       <c r="B113" s="8"/>
       <c r="C113" s="9" t="s">
-        <v>279</v>
+        <v>209</v>
       </c>
     </row>
     <row r="114" spans="1:3" outlineLevel="2">
@@ -3096,35 +3107,35 @@
       </c>
       <c r="B115" s="13"/>
       <c r="C115" s="12" t="s">
-        <v>280</v>
+        <v>210</v>
       </c>
     </row>
     <row r="116" spans="1:3" outlineLevel="3">
       <c r="A116" s="8"/>
       <c r="B116" s="8"/>
       <c r="C116" s="9" t="s">
-        <v>281</v>
+        <v>211</v>
       </c>
     </row>
     <row r="117" spans="1:3" outlineLevel="3">
       <c r="A117" s="8"/>
       <c r="B117" s="8"/>
       <c r="C117" s="9" t="s">
-        <v>282</v>
+        <v>212</v>
       </c>
     </row>
     <row r="118" spans="1:3" outlineLevel="3">
       <c r="A118" s="8"/>
       <c r="B118" s="8"/>
       <c r="C118" s="9" t="s">
-        <v>283</v>
+        <v>213</v>
       </c>
     </row>
     <row r="119" spans="1:3" outlineLevel="3">
       <c r="A119" s="6"/>
       <c r="B119" s="6"/>
       <c r="C119" s="10" t="s">
-        <v>284</v>
+        <v>214</v>
       </c>
     </row>
     <row r="120" spans="1:3" outlineLevel="2">
@@ -3138,35 +3149,35 @@
       </c>
       <c r="B121" s="13"/>
       <c r="C121" s="12" t="s">
-        <v>286</v>
+        <v>216</v>
       </c>
     </row>
     <row r="122" spans="1:3" outlineLevel="3">
       <c r="A122" s="8"/>
       <c r="B122" s="8"/>
       <c r="C122" s="9" t="s">
-        <v>285</v>
+        <v>215</v>
       </c>
     </row>
     <row r="123" spans="1:3" outlineLevel="3">
       <c r="A123" s="8"/>
       <c r="B123" s="8"/>
       <c r="C123" s="9" t="s">
-        <v>287</v>
+        <v>217</v>
       </c>
     </row>
     <row r="124" spans="1:3" outlineLevel="3">
       <c r="A124" s="8"/>
       <c r="B124" s="8"/>
       <c r="C124" s="9" t="s">
-        <v>288</v>
+        <v>218</v>
       </c>
     </row>
     <row r="125" spans="1:3" outlineLevel="3">
       <c r="A125" s="8"/>
       <c r="B125" s="8"/>
       <c r="C125" s="9" t="s">
-        <v>289</v>
+        <v>219</v>
       </c>
     </row>
     <row r="126" spans="1:3" outlineLevel="2">
@@ -3180,21 +3191,21 @@
       </c>
       <c r="B127" s="13"/>
       <c r="C127" s="12" t="s">
-        <v>290</v>
+        <v>220</v>
       </c>
     </row>
     <row r="128" spans="1:3" outlineLevel="3">
       <c r="A128" s="8"/>
       <c r="B128" s="8"/>
       <c r="C128" s="9" t="s">
-        <v>291</v>
+        <v>221</v>
       </c>
     </row>
     <row r="129" spans="1:3" outlineLevel="3">
       <c r="A129" s="8"/>
       <c r="B129" s="8"/>
       <c r="C129" s="9" t="s">
-        <v>292</v>
+        <v>222</v>
       </c>
     </row>
     <row r="130" spans="1:3" outlineLevel="1">
@@ -3208,7 +3219,7 @@
       </c>
       <c r="B131" s="7"/>
       <c r="C131" s="7" t="s">
-        <v>193</v>
+        <v>123</v>
       </c>
     </row>
     <row r="132" spans="1:3" outlineLevel="2">
@@ -3222,49 +3233,49 @@
       </c>
       <c r="B133" s="13"/>
       <c r="C133" s="12" t="s">
-        <v>293</v>
+        <v>223</v>
       </c>
     </row>
     <row r="134" spans="1:3" outlineLevel="3">
       <c r="A134" s="8"/>
       <c r="B134" s="8"/>
       <c r="C134" s="9" t="s">
-        <v>294</v>
+        <v>224</v>
       </c>
     </row>
     <row r="135" spans="1:3" outlineLevel="3">
       <c r="A135" s="8"/>
       <c r="B135" s="8"/>
       <c r="C135" s="9" t="s">
-        <v>295</v>
+        <v>225</v>
       </c>
     </row>
     <row r="136" spans="1:3" outlineLevel="3">
       <c r="A136" s="8"/>
       <c r="B136" s="8"/>
       <c r="C136" s="9" t="s">
-        <v>296</v>
+        <v>226</v>
       </c>
     </row>
     <row r="137" spans="1:3" outlineLevel="3">
       <c r="A137" s="8"/>
       <c r="B137" s="8"/>
       <c r="C137" s="9" t="s">
-        <v>297</v>
+        <v>227</v>
       </c>
     </row>
     <row r="138" spans="1:3" outlineLevel="3">
       <c r="A138" s="8"/>
       <c r="B138" s="8"/>
       <c r="C138" s="9" t="s">
-        <v>298</v>
+        <v>228</v>
       </c>
     </row>
     <row r="139" spans="1:3" outlineLevel="3">
       <c r="A139" s="8"/>
       <c r="B139" s="8"/>
       <c r="C139" s="9" t="s">
-        <v>299</v>
+        <v>229</v>
       </c>
     </row>
     <row r="140" spans="1:3" outlineLevel="2">
@@ -3278,28 +3289,28 @@
       </c>
       <c r="B141" s="13"/>
       <c r="C141" s="12" t="s">
-        <v>300</v>
+        <v>230</v>
       </c>
     </row>
     <row r="142" spans="1:3" outlineLevel="3">
       <c r="A142" s="8"/>
       <c r="B142" s="8"/>
       <c r="C142" s="9" t="s">
-        <v>301</v>
+        <v>231</v>
       </c>
     </row>
     <row r="143" spans="1:3" outlineLevel="3">
       <c r="A143" s="8"/>
       <c r="B143" s="8"/>
       <c r="C143" s="9" t="s">
-        <v>302</v>
+        <v>232</v>
       </c>
     </row>
     <row r="144" spans="1:3" outlineLevel="3">
       <c r="A144" s="8"/>
       <c r="B144" s="8"/>
       <c r="C144" s="9" t="s">
-        <v>303</v>
+        <v>233</v>
       </c>
     </row>
     <row r="145" spans="1:3" outlineLevel="2">
@@ -3313,42 +3324,42 @@
       </c>
       <c r="B146" s="13"/>
       <c r="C146" s="12" t="s">
-        <v>304</v>
+        <v>234</v>
       </c>
     </row>
     <row r="147" spans="1:3" outlineLevel="3">
       <c r="A147" s="8"/>
       <c r="B147" s="8"/>
       <c r="C147" s="9" t="s">
-        <v>305</v>
+        <v>235</v>
       </c>
     </row>
     <row r="148" spans="1:3" outlineLevel="3">
       <c r="A148" s="8"/>
       <c r="B148" s="8"/>
       <c r="C148" s="9" t="s">
-        <v>306</v>
+        <v>236</v>
       </c>
     </row>
     <row r="149" spans="1:3" outlineLevel="3">
       <c r="A149" s="8"/>
       <c r="B149" s="8"/>
       <c r="C149" s="9" t="s">
-        <v>307</v>
+        <v>237</v>
       </c>
     </row>
     <row r="150" spans="1:3" outlineLevel="3">
       <c r="A150" s="8"/>
       <c r="B150" s="8"/>
       <c r="C150" s="9" t="s">
-        <v>308</v>
+        <v>238</v>
       </c>
     </row>
     <row r="151" spans="1:3" outlineLevel="3">
       <c r="A151" s="8"/>
       <c r="B151" s="8"/>
       <c r="C151" s="9" t="s">
-        <v>309</v>
+        <v>239</v>
       </c>
     </row>
     <row r="152" spans="1:3" outlineLevel="2">
@@ -3362,35 +3373,35 @@
       </c>
       <c r="B153" s="13"/>
       <c r="C153" s="12" t="s">
-        <v>310</v>
+        <v>240</v>
       </c>
     </row>
     <row r="154" spans="1:3" outlineLevel="3">
       <c r="A154" s="8"/>
       <c r="B154" s="8"/>
       <c r="C154" s="9" t="s">
-        <v>311</v>
+        <v>241</v>
       </c>
     </row>
     <row r="155" spans="1:3" outlineLevel="3">
       <c r="A155" s="8"/>
       <c r="B155" s="8"/>
       <c r="C155" s="9" t="s">
-        <v>312</v>
+        <v>242</v>
       </c>
     </row>
     <row r="156" spans="1:3" outlineLevel="3">
       <c r="A156" s="8"/>
       <c r="B156" s="8"/>
       <c r="C156" s="9" t="s">
-        <v>313</v>
+        <v>243</v>
       </c>
     </row>
     <row r="157" spans="1:3" outlineLevel="3">
       <c r="A157" s="8"/>
       <c r="B157" s="8"/>
       <c r="C157" s="9" t="s">
-        <v>314</v>
+        <v>244</v>
       </c>
     </row>
     <row r="158" spans="1:3" outlineLevel="2">
@@ -3404,28 +3415,28 @@
       </c>
       <c r="B159" s="13"/>
       <c r="C159" s="12" t="s">
-        <v>315</v>
+        <v>245</v>
       </c>
     </row>
     <row r="160" spans="1:3" outlineLevel="3">
       <c r="A160" s="8"/>
       <c r="B160" s="8"/>
       <c r="C160" s="9" t="s">
-        <v>316</v>
+        <v>246</v>
       </c>
     </row>
     <row r="161" spans="1:3" outlineLevel="3">
       <c r="A161" s="8"/>
       <c r="B161" s="8"/>
       <c r="C161" s="9" t="s">
-        <v>317</v>
+        <v>247</v>
       </c>
     </row>
     <row r="162" spans="1:3" outlineLevel="3">
       <c r="A162" s="8"/>
       <c r="B162" s="8"/>
       <c r="C162" s="9" t="s">
-        <v>318</v>
+        <v>248</v>
       </c>
     </row>
     <row r="163" spans="1:3" outlineLevel="2">
@@ -3439,28 +3450,28 @@
       </c>
       <c r="B164" s="13"/>
       <c r="C164" s="12" t="s">
-        <v>319</v>
+        <v>249</v>
       </c>
     </row>
     <row r="165" spans="1:3" outlineLevel="3">
       <c r="A165" s="8"/>
       <c r="B165" s="8"/>
       <c r="C165" s="9" t="s">
-        <v>320</v>
+        <v>250</v>
       </c>
     </row>
     <row r="166" spans="1:3" outlineLevel="3">
       <c r="A166" s="8"/>
       <c r="B166" s="8"/>
       <c r="C166" s="9" t="s">
-        <v>321</v>
+        <v>251</v>
       </c>
     </row>
     <row r="167" spans="1:3" outlineLevel="3">
       <c r="A167" s="8"/>
       <c r="B167" s="8"/>
       <c r="C167" s="9" t="s">
-        <v>322</v>
+        <v>252</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -3502,49 +3513,49 @@
       </c>
       <c r="B173" s="13"/>
       <c r="C173" s="12" t="s">
-        <v>324</v>
+        <v>254</v>
       </c>
     </row>
     <row r="174" spans="1:3" outlineLevel="3">
       <c r="A174" s="8"/>
       <c r="B174" s="8"/>
       <c r="C174" s="9" t="s">
-        <v>323</v>
+        <v>253</v>
       </c>
     </row>
     <row r="175" spans="1:3" outlineLevel="3">
       <c r="A175" s="8"/>
       <c r="B175" s="8"/>
       <c r="C175" s="9" t="s">
-        <v>325</v>
+        <v>255</v>
       </c>
     </row>
     <row r="176" spans="1:3" outlineLevel="3">
       <c r="A176" s="8"/>
       <c r="B176" s="8"/>
       <c r="C176" s="9" t="s">
-        <v>326</v>
+        <v>256</v>
       </c>
     </row>
     <row r="177" spans="1:3" outlineLevel="3">
       <c r="A177" s="8"/>
       <c r="B177" s="8"/>
       <c r="C177" s="9" t="s">
-        <v>327</v>
+        <v>257</v>
       </c>
     </row>
     <row r="178" spans="1:3" outlineLevel="3">
       <c r="A178" s="8"/>
       <c r="B178" s="8"/>
       <c r="C178" s="9" t="s">
-        <v>328</v>
+        <v>258</v>
       </c>
     </row>
     <row r="179" spans="1:3" outlineLevel="3">
       <c r="A179" s="8"/>
       <c r="B179" s="8"/>
       <c r="C179" s="9" t="s">
-        <v>329</v>
+        <v>259</v>
       </c>
     </row>
     <row r="180" spans="1:3" outlineLevel="2">
@@ -3558,70 +3569,70 @@
       </c>
       <c r="B181" s="13"/>
       <c r="C181" s="12" t="s">
-        <v>330</v>
+        <v>260</v>
       </c>
     </row>
     <row r="182" spans="1:3" outlineLevel="3">
       <c r="A182" s="8"/>
       <c r="B182" s="8"/>
       <c r="C182" s="9" t="s">
-        <v>331</v>
+        <v>261</v>
       </c>
     </row>
     <row r="183" spans="1:3" outlineLevel="3">
       <c r="A183" s="8"/>
       <c r="B183" s="8"/>
       <c r="C183" s="9" t="s">
-        <v>332</v>
+        <v>262</v>
       </c>
     </row>
     <row r="184" spans="1:3" outlineLevel="3">
       <c r="A184" s="8"/>
       <c r="B184" s="8"/>
       <c r="C184" s="9" t="s">
-        <v>333</v>
+        <v>263</v>
       </c>
     </row>
     <row r="185" spans="1:3" outlineLevel="3">
       <c r="A185" s="8"/>
       <c r="B185" s="8"/>
       <c r="C185" s="9" t="s">
-        <v>334</v>
+        <v>264</v>
       </c>
     </row>
     <row r="186" spans="1:3" outlineLevel="3">
       <c r="A186" s="8"/>
       <c r="B186" s="8"/>
       <c r="C186" s="9" t="s">
-        <v>335</v>
+        <v>265</v>
       </c>
     </row>
     <row r="187" spans="1:3" outlineLevel="3">
       <c r="A187" s="8"/>
       <c r="B187" s="8"/>
       <c r="C187" s="9" t="s">
-        <v>336</v>
+        <v>266</v>
       </c>
     </row>
     <row r="188" spans="1:3" outlineLevel="3">
       <c r="A188" s="8"/>
       <c r="B188" s="8"/>
       <c r="C188" s="9" t="s">
-        <v>337</v>
+        <v>267</v>
       </c>
     </row>
     <row r="189" spans="1:3" outlineLevel="3">
       <c r="A189" s="8"/>
       <c r="B189" s="8"/>
       <c r="C189" s="9" t="s">
-        <v>338</v>
+        <v>268</v>
       </c>
     </row>
     <row r="190" spans="1:3" outlineLevel="3">
       <c r="A190" s="8"/>
       <c r="B190" s="8"/>
       <c r="C190" s="9" t="s">
-        <v>339</v>
+        <v>269</v>
       </c>
     </row>
     <row r="191" spans="1:3" outlineLevel="2">
@@ -3635,35 +3646,35 @@
       </c>
       <c r="B192" s="13"/>
       <c r="C192" s="12" t="s">
-        <v>340</v>
+        <v>270</v>
       </c>
     </row>
     <row r="193" spans="1:3" outlineLevel="3">
       <c r="A193" s="8"/>
       <c r="B193" s="8"/>
       <c r="C193" s="9" t="s">
-        <v>341</v>
+        <v>271</v>
       </c>
     </row>
     <row r="194" spans="1:3" outlineLevel="3">
       <c r="A194" s="8"/>
       <c r="B194" s="8"/>
       <c r="C194" s="9" t="s">
-        <v>342</v>
+        <v>272</v>
       </c>
     </row>
     <row r="195" spans="1:3" outlineLevel="3">
       <c r="A195" s="8"/>
       <c r="B195" s="8"/>
       <c r="C195" s="9" t="s">
-        <v>343</v>
+        <v>273</v>
       </c>
     </row>
     <row r="196" spans="1:3" outlineLevel="3">
       <c r="A196" s="8"/>
       <c r="B196" s="8"/>
       <c r="C196" s="9" t="s">
-        <v>344</v>
+        <v>274</v>
       </c>
     </row>
     <row r="197" spans="1:3" outlineLevel="2">
@@ -3677,49 +3688,49 @@
       </c>
       <c r="B198" s="13"/>
       <c r="C198" s="12" t="s">
-        <v>345</v>
+        <v>275</v>
       </c>
     </row>
     <row r="199" spans="1:3" outlineLevel="3">
       <c r="A199" s="8"/>
       <c r="B199" s="8"/>
       <c r="C199" s="9" t="s">
-        <v>346</v>
+        <v>276</v>
       </c>
     </row>
     <row r="200" spans="1:3" outlineLevel="3">
       <c r="A200" s="8"/>
       <c r="B200" s="8"/>
       <c r="C200" s="9" t="s">
-        <v>347</v>
+        <v>277</v>
       </c>
     </row>
     <row r="201" spans="1:3" outlineLevel="3">
       <c r="A201" s="8"/>
       <c r="B201" s="8"/>
       <c r="C201" s="9" t="s">
-        <v>348</v>
+        <v>278</v>
       </c>
     </row>
     <row r="202" spans="1:3" outlineLevel="3">
       <c r="A202" s="8"/>
       <c r="B202" s="8"/>
       <c r="C202" s="9" t="s">
-        <v>349</v>
+        <v>279</v>
       </c>
     </row>
     <row r="203" spans="1:3" outlineLevel="3">
       <c r="A203" s="8"/>
       <c r="B203" s="8"/>
       <c r="C203" s="9" t="s">
-        <v>350</v>
+        <v>280</v>
       </c>
     </row>
     <row r="204" spans="1:3" outlineLevel="3">
       <c r="A204" s="8"/>
       <c r="B204" s="8"/>
       <c r="C204" s="9" t="s">
-        <v>351</v>
+        <v>281</v>
       </c>
     </row>
     <row r="205" spans="1:3" outlineLevel="2">
@@ -3733,49 +3744,49 @@
       </c>
       <c r="B206" s="13"/>
       <c r="C206" s="12" t="s">
-        <v>352</v>
+        <v>282</v>
       </c>
     </row>
     <row r="207" spans="1:3" outlineLevel="3">
       <c r="A207" s="8"/>
       <c r="B207" s="8"/>
       <c r="C207" s="9" t="s">
-        <v>353</v>
+        <v>283</v>
       </c>
     </row>
     <row r="208" spans="1:3" outlineLevel="3">
       <c r="A208" s="8"/>
       <c r="B208" s="8"/>
       <c r="C208" s="9" t="s">
-        <v>354</v>
+        <v>284</v>
       </c>
     </row>
     <row r="209" spans="1:3" outlineLevel="3">
       <c r="A209" s="8"/>
       <c r="B209" s="8"/>
       <c r="C209" s="9" t="s">
-        <v>355</v>
+        <v>285</v>
       </c>
     </row>
     <row r="210" spans="1:3" outlineLevel="3">
       <c r="A210" s="8"/>
       <c r="B210" s="8"/>
       <c r="C210" s="9" t="s">
-        <v>356</v>
+        <v>286</v>
       </c>
     </row>
     <row r="211" spans="1:3" outlineLevel="3">
       <c r="A211" s="8"/>
       <c r="B211" s="8"/>
       <c r="C211" s="9" t="s">
-        <v>357</v>
+        <v>287</v>
       </c>
     </row>
     <row r="212" spans="1:3" outlineLevel="3">
       <c r="A212" s="8"/>
       <c r="B212" s="8"/>
       <c r="C212" s="9" t="s">
-        <v>358</v>
+        <v>288</v>
       </c>
     </row>
     <row r="213" spans="1:3" outlineLevel="1">
@@ -3803,63 +3814,63 @@
       </c>
       <c r="B216" s="13"/>
       <c r="C216" s="12" t="s">
-        <v>359</v>
+        <v>289</v>
       </c>
     </row>
     <row r="217" spans="1:3" outlineLevel="3">
       <c r="A217" s="6"/>
       <c r="B217" s="6"/>
       <c r="C217" s="10" t="s">
-        <v>360</v>
+        <v>290</v>
       </c>
     </row>
     <row r="218" spans="1:3" outlineLevel="3">
       <c r="A218" s="6"/>
       <c r="B218" s="6"/>
       <c r="C218" s="10" t="s">
-        <v>361</v>
+        <v>291</v>
       </c>
     </row>
     <row r="219" spans="1:3" outlineLevel="3">
       <c r="A219" s="6"/>
       <c r="B219" s="6"/>
       <c r="C219" s="10" t="s">
-        <v>362</v>
+        <v>292</v>
       </c>
     </row>
     <row r="220" spans="1:3" outlineLevel="3">
       <c r="A220" s="6"/>
       <c r="B220" s="6"/>
       <c r="C220" s="10" t="s">
-        <v>363</v>
+        <v>293</v>
       </c>
     </row>
     <row r="221" spans="1:3" outlineLevel="3">
       <c r="A221" s="6"/>
       <c r="B221" s="6"/>
       <c r="C221" s="10" t="s">
-        <v>364</v>
+        <v>294</v>
       </c>
     </row>
     <row r="222" spans="1:3" outlineLevel="3">
       <c r="A222" s="6"/>
       <c r="B222" s="6"/>
       <c r="C222" s="10" t="s">
-        <v>365</v>
+        <v>295</v>
       </c>
     </row>
     <row r="223" spans="1:3" outlineLevel="3">
       <c r="A223" s="6"/>
       <c r="B223" s="6"/>
       <c r="C223" s="10" t="s">
-        <v>366</v>
+        <v>296</v>
       </c>
     </row>
     <row r="224" spans="1:3" outlineLevel="3">
       <c r="A224" s="6"/>
       <c r="B224" s="6"/>
       <c r="C224" s="10" t="s">
-        <v>367</v>
+        <v>297</v>
       </c>
     </row>
     <row r="225" spans="1:3" outlineLevel="2">
@@ -3873,42 +3884,42 @@
       </c>
       <c r="B226" s="13"/>
       <c r="C226" s="12" t="s">
-        <v>368</v>
+        <v>298</v>
       </c>
     </row>
     <row r="227" spans="1:3" outlineLevel="3">
       <c r="A227" s="6"/>
       <c r="B227" s="6"/>
       <c r="C227" s="10" t="s">
-        <v>369</v>
+        <v>299</v>
       </c>
     </row>
     <row r="228" spans="1:3" outlineLevel="3">
       <c r="A228" s="6"/>
       <c r="B228" s="6"/>
       <c r="C228" s="10" t="s">
-        <v>370</v>
+        <v>300</v>
       </c>
     </row>
     <row r="229" spans="1:3" outlineLevel="3">
       <c r="A229" s="6"/>
       <c r="B229" s="6"/>
       <c r="C229" s="10" t="s">
-        <v>371</v>
+        <v>301</v>
       </c>
     </row>
     <row r="230" spans="1:3" outlineLevel="3">
       <c r="A230" s="6"/>
       <c r="B230" s="6"/>
       <c r="C230" s="10" t="s">
-        <v>372</v>
+        <v>302</v>
       </c>
     </row>
     <row r="231" spans="1:3" outlineLevel="3">
       <c r="A231" s="6"/>
       <c r="B231" s="6"/>
       <c r="C231" s="10" t="s">
-        <v>373</v>
+        <v>303</v>
       </c>
     </row>
     <row r="232" spans="1:3" outlineLevel="2">
@@ -3922,42 +3933,42 @@
       </c>
       <c r="B233" s="13"/>
       <c r="C233" s="12" t="s">
-        <v>374</v>
+        <v>304</v>
       </c>
     </row>
     <row r="234" spans="1:3" outlineLevel="3">
       <c r="A234" s="6"/>
       <c r="B234" s="6"/>
       <c r="C234" s="10" t="s">
-        <v>375</v>
+        <v>305</v>
       </c>
     </row>
     <row r="235" spans="1:3" outlineLevel="3">
       <c r="A235" s="6"/>
       <c r="B235" s="6"/>
       <c r="C235" s="10" t="s">
-        <v>376</v>
+        <v>306</v>
       </c>
     </row>
     <row r="236" spans="1:3" outlineLevel="3">
       <c r="A236" s="6"/>
       <c r="B236" s="6"/>
       <c r="C236" s="10" t="s">
-        <v>377</v>
+        <v>307</v>
       </c>
     </row>
     <row r="237" spans="1:3" outlineLevel="3">
       <c r="A237" s="6"/>
       <c r="B237" s="6"/>
       <c r="C237" s="10" t="s">
-        <v>378</v>
+        <v>308</v>
       </c>
     </row>
     <row r="238" spans="1:3" outlineLevel="3">
       <c r="A238" s="6"/>
       <c r="B238" s="6"/>
       <c r="C238" s="10" t="s">
-        <v>379</v>
+        <v>309</v>
       </c>
     </row>
     <row r="239" spans="1:3" outlineLevel="2">
@@ -3971,28 +3982,28 @@
       </c>
       <c r="B240" s="13"/>
       <c r="C240" s="12" t="s">
-        <v>380</v>
+        <v>310</v>
       </c>
     </row>
     <row r="241" spans="1:3" outlineLevel="3">
       <c r="A241" s="6"/>
       <c r="B241" s="6"/>
       <c r="C241" s="10" t="s">
-        <v>381</v>
+        <v>311</v>
       </c>
     </row>
     <row r="242" spans="1:3" outlineLevel="3">
       <c r="A242" s="6"/>
       <c r="B242" s="6"/>
       <c r="C242" s="10" t="s">
-        <v>382</v>
+        <v>312</v>
       </c>
     </row>
     <row r="243" spans="1:3" outlineLevel="3">
       <c r="A243" s="6"/>
       <c r="B243" s="6"/>
       <c r="C243" s="10" t="s">
-        <v>383</v>
+        <v>313</v>
       </c>
     </row>
     <row r="244" spans="1:3" outlineLevel="2">
@@ -4006,35 +4017,35 @@
       </c>
       <c r="B245" s="13"/>
       <c r="C245" s="12" t="s">
-        <v>384</v>
+        <v>314</v>
       </c>
     </row>
     <row r="246" spans="1:3" outlineLevel="3">
       <c r="A246" s="6"/>
       <c r="B246" s="6"/>
       <c r="C246" s="10" t="s">
-        <v>386</v>
+        <v>316</v>
       </c>
     </row>
     <row r="247" spans="1:3" outlineLevel="3">
       <c r="A247" s="6"/>
       <c r="B247" s="6"/>
       <c r="C247" s="10" t="s">
-        <v>385</v>
+        <v>315</v>
       </c>
     </row>
     <row r="248" spans="1:3" outlineLevel="3">
       <c r="A248" s="6"/>
       <c r="B248" s="6"/>
       <c r="C248" s="10" t="s">
-        <v>387</v>
+        <v>317</v>
       </c>
     </row>
     <row r="249" spans="1:3" outlineLevel="3">
       <c r="A249" s="6"/>
       <c r="B249" s="6"/>
       <c r="C249" s="10" t="s">
-        <v>388</v>
+        <v>318</v>
       </c>
     </row>
     <row r="250" spans="1:3" outlineLevel="2">
@@ -4048,28 +4059,28 @@
       </c>
       <c r="B251" s="13"/>
       <c r="C251" s="12" t="s">
-        <v>389</v>
+        <v>319</v>
       </c>
     </row>
     <row r="252" spans="1:3" outlineLevel="3">
       <c r="A252" s="6"/>
       <c r="B252" s="6"/>
       <c r="C252" s="10" t="s">
-        <v>390</v>
+        <v>320</v>
       </c>
     </row>
     <row r="253" spans="1:3" outlineLevel="3">
       <c r="A253" s="6"/>
       <c r="B253" s="6"/>
       <c r="C253" s="10" t="s">
-        <v>391</v>
+        <v>321</v>
       </c>
     </row>
     <row r="254" spans="1:3" outlineLevel="3">
       <c r="A254" s="6"/>
       <c r="B254" s="6"/>
       <c r="C254" s="10" t="s">
-        <v>392</v>
+        <v>322</v>
       </c>
     </row>
     <row r="255" spans="1:3" outlineLevel="2">
@@ -4083,42 +4094,42 @@
       </c>
       <c r="B256" s="13"/>
       <c r="C256" s="12" t="s">
-        <v>393</v>
+        <v>323</v>
       </c>
     </row>
     <row r="257" spans="1:3" outlineLevel="3">
       <c r="A257" s="6"/>
       <c r="B257" s="6"/>
       <c r="C257" s="10" t="s">
-        <v>394</v>
+        <v>324</v>
       </c>
     </row>
     <row r="258" spans="1:3" outlineLevel="3">
       <c r="A258" s="6"/>
       <c r="B258" s="6"/>
       <c r="C258" s="10" t="s">
-        <v>395</v>
+        <v>325</v>
       </c>
     </row>
     <row r="259" spans="1:3" outlineLevel="3">
       <c r="A259" s="6"/>
       <c r="B259" s="6"/>
       <c r="C259" s="10" t="s">
-        <v>396</v>
+        <v>326</v>
       </c>
     </row>
     <row r="260" spans="1:3" outlineLevel="3">
       <c r="A260" s="6"/>
       <c r="B260" s="6"/>
       <c r="C260" s="10" t="s">
-        <v>397</v>
+        <v>327</v>
       </c>
     </row>
     <row r="261" spans="1:3" outlineLevel="3">
       <c r="A261" s="6"/>
       <c r="B261" s="6"/>
       <c r="C261" s="10" t="s">
-        <v>398</v>
+        <v>328</v>
       </c>
     </row>
     <row r="262" spans="1:3" outlineLevel="2">
@@ -4132,35 +4143,35 @@
       </c>
       <c r="B263" s="13"/>
       <c r="C263" s="12" t="s">
-        <v>399</v>
+        <v>329</v>
       </c>
     </row>
     <row r="264" spans="1:3" outlineLevel="3">
       <c r="A264" s="6"/>
       <c r="B264" s="6"/>
       <c r="C264" s="10" t="s">
-        <v>400</v>
+        <v>330</v>
       </c>
     </row>
     <row r="265" spans="1:3" outlineLevel="3">
       <c r="A265" s="6"/>
       <c r="B265" s="6"/>
       <c r="C265" s="10" t="s">
-        <v>401</v>
+        <v>331</v>
       </c>
     </row>
     <row r="266" spans="1:3" outlineLevel="3">
       <c r="A266" s="6"/>
       <c r="B266" s="6"/>
       <c r="C266" s="10" t="s">
-        <v>402</v>
+        <v>332</v>
       </c>
     </row>
     <row r="267" spans="1:3" outlineLevel="3">
       <c r="A267" s="6"/>
       <c r="B267" s="6"/>
       <c r="C267" s="10" t="s">
-        <v>403</v>
+        <v>333</v>
       </c>
     </row>
     <row r="268" spans="1:3" outlineLevel="2">
@@ -4174,35 +4185,35 @@
       </c>
       <c r="B269" s="13"/>
       <c r="C269" s="12" t="s">
-        <v>404</v>
+        <v>334</v>
       </c>
     </row>
     <row r="270" spans="1:3" outlineLevel="3">
       <c r="A270" s="6"/>
       <c r="B270" s="6"/>
       <c r="C270" s="10" t="s">
-        <v>405</v>
+        <v>335</v>
       </c>
     </row>
     <row r="271" spans="1:3" outlineLevel="3">
       <c r="A271" s="6"/>
       <c r="B271" s="6"/>
       <c r="C271" s="10" t="s">
-        <v>406</v>
+        <v>336</v>
       </c>
     </row>
     <row r="272" spans="1:3" outlineLevel="3">
       <c r="A272" s="6"/>
       <c r="B272" s="6"/>
       <c r="C272" s="10" t="s">
-        <v>407</v>
+        <v>337</v>
       </c>
     </row>
     <row r="273" spans="1:3" outlineLevel="3">
       <c r="A273" s="6"/>
       <c r="B273" s="6"/>
       <c r="C273" s="10" t="s">
-        <v>408</v>
+        <v>338</v>
       </c>
     </row>
     <row r="274" spans="1:3" outlineLevel="2">
@@ -4216,35 +4227,35 @@
       </c>
       <c r="B275" s="13"/>
       <c r="C275" s="12" t="s">
-        <v>409</v>
+        <v>339</v>
       </c>
     </row>
     <row r="276" spans="1:3" outlineLevel="3">
       <c r="A276" s="6"/>
       <c r="B276" s="6"/>
       <c r="C276" s="10" t="s">
-        <v>410</v>
+        <v>340</v>
       </c>
     </row>
     <row r="277" spans="1:3" outlineLevel="3">
       <c r="A277" s="6"/>
       <c r="B277" s="6"/>
       <c r="C277" s="10" t="s">
-        <v>411</v>
+        <v>341</v>
       </c>
     </row>
     <row r="278" spans="1:3" outlineLevel="3">
       <c r="A278" s="6"/>
       <c r="B278" s="6"/>
       <c r="C278" s="10" t="s">
-        <v>412</v>
+        <v>342</v>
       </c>
     </row>
     <row r="279" spans="1:3" outlineLevel="3">
       <c r="A279" s="6"/>
       <c r="B279" s="6"/>
       <c r="C279" s="10" t="s">
-        <v>413</v>
+        <v>343</v>
       </c>
     </row>
     <row r="280" spans="1:3" outlineLevel="1">
@@ -4272,7 +4283,7 @@
       </c>
       <c r="B283" s="13"/>
       <c r="C283" s="12" t="s">
-        <v>415</v>
+        <v>345</v>
       </c>
     </row>
     <row r="284" spans="1:3" outlineLevel="2">
@@ -4286,7 +4297,7 @@
       </c>
       <c r="B285" s="13"/>
       <c r="C285" s="12" t="s">
-        <v>414</v>
+        <v>344</v>
       </c>
     </row>
     <row r="286" spans="1:3" outlineLevel="2">
@@ -4300,7 +4311,7 @@
       </c>
       <c r="B287" s="13"/>
       <c r="C287" s="12" t="s">
-        <v>416</v>
+        <v>346</v>
       </c>
     </row>
     <row r="288" spans="1:3">
@@ -4342,21 +4353,21 @@
       </c>
       <c r="B293" s="13"/>
       <c r="C293" s="12" t="s">
-        <v>417</v>
+        <v>347</v>
       </c>
     </row>
     <row r="294" spans="1:3" outlineLevel="3">
       <c r="A294" s="8"/>
       <c r="B294" s="8"/>
       <c r="C294" s="9" t="s">
-        <v>418</v>
+        <v>348</v>
       </c>
     </row>
     <row r="295" spans="1:3" outlineLevel="3">
       <c r="A295" s="8"/>
       <c r="B295" s="8"/>
       <c r="C295" s="9" t="s">
-        <v>419</v>
+        <v>349</v>
       </c>
     </row>
     <row r="296" spans="1:3" outlineLevel="2">
@@ -4370,14 +4381,14 @@
       </c>
       <c r="B297" s="13"/>
       <c r="C297" s="12" t="s">
-        <v>420</v>
+        <v>350</v>
       </c>
     </row>
     <row r="298" spans="1:3" outlineLevel="3">
       <c r="A298" s="8"/>
       <c r="B298" s="8"/>
       <c r="C298" s="9" t="s">
-        <v>421</v>
+        <v>351</v>
       </c>
     </row>
     <row r="299" spans="1:3" outlineLevel="2">
@@ -4391,35 +4402,35 @@
       </c>
       <c r="B300" s="13"/>
       <c r="C300" s="12" t="s">
-        <v>422</v>
+        <v>352</v>
       </c>
     </row>
     <row r="301" spans="1:3" outlineLevel="3">
       <c r="A301" s="8"/>
       <c r="B301" s="8"/>
       <c r="C301" s="9" t="s">
-        <v>423</v>
+        <v>353</v>
       </c>
     </row>
     <row r="302" spans="1:3" outlineLevel="3">
       <c r="A302" s="8"/>
       <c r="B302" s="8"/>
       <c r="C302" s="9" t="s">
-        <v>424</v>
+        <v>354</v>
       </c>
     </row>
     <row r="303" spans="1:3" outlineLevel="3">
       <c r="A303" s="8"/>
       <c r="B303" s="8"/>
       <c r="C303" s="9" t="s">
-        <v>425</v>
+        <v>355</v>
       </c>
     </row>
     <row r="304" spans="1:3" outlineLevel="3">
       <c r="A304" s="8"/>
       <c r="B304" s="8"/>
       <c r="C304" s="9" t="s">
-        <v>426</v>
+        <v>356</v>
       </c>
     </row>
     <row r="305" spans="1:3" outlineLevel="2">
@@ -4433,21 +4444,21 @@
       </c>
       <c r="B306" s="13"/>
       <c r="C306" s="12" t="s">
-        <v>427</v>
+        <v>357</v>
       </c>
     </row>
     <row r="307" spans="1:3" outlineLevel="3">
       <c r="A307" s="8"/>
       <c r="B307" s="8"/>
       <c r="C307" s="9" t="s">
-        <v>428</v>
+        <v>358</v>
       </c>
     </row>
     <row r="308" spans="1:3" outlineLevel="3">
       <c r="A308" s="8"/>
       <c r="B308" s="8"/>
       <c r="C308" s="9" t="s">
-        <v>429</v>
+        <v>359</v>
       </c>
     </row>
     <row r="309" spans="1:3" outlineLevel="2">
@@ -4461,28 +4472,28 @@
       </c>
       <c r="B310" s="13"/>
       <c r="C310" s="12" t="s">
-        <v>430</v>
+        <v>360</v>
       </c>
     </row>
     <row r="311" spans="1:3" outlineLevel="3">
       <c r="A311" s="8"/>
       <c r="B311" s="8"/>
       <c r="C311" s="9" t="s">
-        <v>431</v>
+        <v>361</v>
       </c>
     </row>
     <row r="312" spans="1:3" outlineLevel="3">
       <c r="A312" s="8"/>
       <c r="B312" s="8"/>
       <c r="C312" s="9" t="s">
-        <v>432</v>
+        <v>362</v>
       </c>
     </row>
     <row r="313" spans="1:3" outlineLevel="3">
       <c r="A313" s="8"/>
       <c r="B313" s="8"/>
       <c r="C313" s="9" t="s">
-        <v>433</v>
+        <v>363</v>
       </c>
     </row>
     <row r="314" spans="1:3" outlineLevel="2">
@@ -4496,28 +4507,28 @@
       </c>
       <c r="B315" s="13"/>
       <c r="C315" s="12" t="s">
-        <v>434</v>
+        <v>364</v>
       </c>
     </row>
     <row r="316" spans="1:3" outlineLevel="3">
       <c r="A316" s="8"/>
       <c r="B316" s="8"/>
       <c r="C316" s="9" t="s">
-        <v>435</v>
+        <v>365</v>
       </c>
     </row>
     <row r="317" spans="1:3" outlineLevel="3">
       <c r="A317" s="8"/>
       <c r="B317" s="8"/>
       <c r="C317" s="9" t="s">
-        <v>436</v>
+        <v>366</v>
       </c>
     </row>
     <row r="318" spans="1:3" outlineLevel="3">
       <c r="A318" s="8"/>
       <c r="B318" s="8"/>
       <c r="C318" s="9" t="s">
-        <v>437</v>
+        <v>367</v>
       </c>
     </row>
     <row r="319" spans="1:3" outlineLevel="2">
@@ -4531,35 +4542,35 @@
       </c>
       <c r="B320" s="13"/>
       <c r="C320" s="12" t="s">
-        <v>438</v>
+        <v>368</v>
       </c>
     </row>
     <row r="321" spans="1:3" outlineLevel="3">
       <c r="A321" s="8"/>
       <c r="B321" s="8"/>
       <c r="C321" s="9" t="s">
-        <v>439</v>
+        <v>369</v>
       </c>
     </row>
     <row r="322" spans="1:3" outlineLevel="3">
       <c r="A322" s="8"/>
       <c r="B322" s="8"/>
       <c r="C322" s="9" t="s">
-        <v>440</v>
+        <v>370</v>
       </c>
     </row>
     <row r="323" spans="1:3" outlineLevel="3">
       <c r="A323" s="8"/>
       <c r="B323" s="8"/>
       <c r="C323" s="9" t="s">
-        <v>441</v>
+        <v>371</v>
       </c>
     </row>
     <row r="324" spans="1:3" outlineLevel="3">
       <c r="A324" s="8"/>
       <c r="B324" s="8"/>
       <c r="C324" s="9" t="s">
-        <v>442</v>
+        <v>372</v>
       </c>
     </row>
     <row r="325" spans="1:3" outlineLevel="1">
@@ -4587,70 +4598,70 @@
       </c>
       <c r="B328" s="13"/>
       <c r="C328" s="14" t="s">
-        <v>443</v>
+        <v>373</v>
       </c>
     </row>
     <row r="329" spans="1:3" outlineLevel="3">
       <c r="A329" s="8"/>
       <c r="B329" s="8"/>
       <c r="C329" s="9" t="s">
-        <v>444</v>
+        <v>374</v>
       </c>
     </row>
     <row r="330" spans="1:3" outlineLevel="3">
       <c r="A330" s="8"/>
       <c r="B330" s="8"/>
       <c r="C330" s="9" t="s">
-        <v>445</v>
+        <v>375</v>
       </c>
     </row>
     <row r="331" spans="1:3" outlineLevel="3">
       <c r="A331" s="8"/>
       <c r="B331" s="8"/>
       <c r="C331" s="9" t="s">
-        <v>446</v>
+        <v>376</v>
       </c>
     </row>
     <row r="332" spans="1:3" outlineLevel="3">
       <c r="A332" s="8"/>
       <c r="B332" s="8"/>
       <c r="C332" s="9" t="s">
-        <v>447</v>
+        <v>377</v>
       </c>
     </row>
     <row r="333" spans="1:3" outlineLevel="3">
       <c r="A333" s="8"/>
       <c r="B333" s="8"/>
       <c r="C333" s="9" t="s">
-        <v>448</v>
+        <v>378</v>
       </c>
     </row>
     <row r="334" spans="1:3" outlineLevel="3">
       <c r="A334" s="8"/>
       <c r="B334" s="8"/>
       <c r="C334" s="9" t="s">
-        <v>449</v>
+        <v>379</v>
       </c>
     </row>
     <row r="335" spans="1:3" outlineLevel="3">
       <c r="A335" s="8"/>
       <c r="B335" s="8"/>
       <c r="C335" s="9" t="s">
-        <v>450</v>
+        <v>380</v>
       </c>
     </row>
     <row r="336" spans="1:3" outlineLevel="3">
       <c r="A336" s="8"/>
       <c r="B336" s="8"/>
       <c r="C336" s="9" t="s">
-        <v>451</v>
+        <v>381</v>
       </c>
     </row>
     <row r="337" spans="1:3" outlineLevel="3">
       <c r="A337" s="8"/>
       <c r="B337" s="8"/>
       <c r="C337" s="9" t="s">
-        <v>452</v>
+        <v>382</v>
       </c>
     </row>
     <row r="338" spans="1:3" outlineLevel="2">
@@ -4664,49 +4675,49 @@
       </c>
       <c r="B339" s="13"/>
       <c r="C339" s="12" t="s">
-        <v>453</v>
+        <v>383</v>
       </c>
     </row>
     <row r="340" spans="1:3" outlineLevel="3">
       <c r="A340" s="8"/>
       <c r="B340" s="8"/>
       <c r="C340" s="9" t="s">
-        <v>454</v>
+        <v>384</v>
       </c>
     </row>
     <row r="341" spans="1:3" outlineLevel="3">
       <c r="A341" s="8"/>
       <c r="B341" s="8"/>
       <c r="C341" s="9" t="s">
-        <v>455</v>
+        <v>385</v>
       </c>
     </row>
     <row r="342" spans="1:3" outlineLevel="3">
       <c r="A342" s="8"/>
       <c r="B342" s="8"/>
       <c r="C342" s="9" t="s">
-        <v>456</v>
+        <v>386</v>
       </c>
     </row>
     <row r="343" spans="1:3" outlineLevel="3">
       <c r="A343" s="8"/>
       <c r="B343" s="8"/>
       <c r="C343" s="9" t="s">
-        <v>457</v>
+        <v>387</v>
       </c>
     </row>
     <row r="344" spans="1:3" outlineLevel="3">
       <c r="A344" s="8"/>
       <c r="B344" s="8"/>
       <c r="C344" s="9" t="s">
-        <v>458</v>
+        <v>388</v>
       </c>
     </row>
     <row r="345" spans="1:3" outlineLevel="3">
       <c r="A345" s="8"/>
       <c r="B345" s="8"/>
       <c r="C345" s="9" t="s">
-        <v>459</v>
+        <v>389</v>
       </c>
     </row>
     <row r="346" spans="1:3" outlineLevel="2">
@@ -4720,28 +4731,28 @@
       </c>
       <c r="B347" s="13"/>
       <c r="C347" s="12" t="s">
-        <v>460</v>
+        <v>390</v>
       </c>
     </row>
     <row r="348" spans="1:3" outlineLevel="3">
       <c r="A348" s="8"/>
       <c r="B348" s="8"/>
       <c r="C348" s="9" t="s">
-        <v>461</v>
+        <v>391</v>
       </c>
     </row>
     <row r="349" spans="1:3" outlineLevel="3">
       <c r="A349" s="8"/>
       <c r="B349" s="8"/>
       <c r="C349" s="9" t="s">
-        <v>462</v>
+        <v>392</v>
       </c>
     </row>
     <row r="350" spans="1:3" outlineLevel="3">
       <c r="A350" s="8"/>
       <c r="B350" s="8"/>
       <c r="C350" s="9" t="s">
-        <v>463</v>
+        <v>393</v>
       </c>
     </row>
     <row r="351" spans="1:3" outlineLevel="2">
@@ -4755,42 +4766,42 @@
       </c>
       <c r="B352" s="13"/>
       <c r="C352" s="12" t="s">
-        <v>464</v>
+        <v>394</v>
       </c>
     </row>
     <row r="353" spans="1:3" outlineLevel="3">
       <c r="A353" s="8"/>
       <c r="B353" s="8"/>
       <c r="C353" s="9" t="s">
-        <v>465</v>
+        <v>395</v>
       </c>
     </row>
     <row r="354" spans="1:3" outlineLevel="3">
       <c r="A354" s="8"/>
       <c r="B354" s="8"/>
       <c r="C354" s="9" t="s">
-        <v>466</v>
+        <v>396</v>
       </c>
     </row>
     <row r="355" spans="1:3" outlineLevel="3">
       <c r="A355" s="8"/>
       <c r="B355" s="8"/>
       <c r="C355" s="9" t="s">
-        <v>467</v>
+        <v>397</v>
       </c>
     </row>
     <row r="356" spans="1:3" outlineLevel="3">
       <c r="A356" s="8"/>
       <c r="B356" s="8"/>
       <c r="C356" s="9" t="s">
-        <v>468</v>
+        <v>398</v>
       </c>
     </row>
     <row r="357" spans="1:3" outlineLevel="3">
       <c r="A357" s="8"/>
       <c r="B357" s="8"/>
       <c r="C357" s="9" t="s">
-        <v>469</v>
+        <v>399</v>
       </c>
     </row>
     <row r="358" spans="1:3" outlineLevel="2">
@@ -4804,28 +4815,28 @@
       </c>
       <c r="B359" s="13"/>
       <c r="C359" s="12" t="s">
-        <v>470</v>
+        <v>400</v>
       </c>
     </row>
     <row r="360" spans="1:3" outlineLevel="3">
       <c r="A360" s="8"/>
       <c r="B360" s="8"/>
       <c r="C360" s="9" t="s">
-        <v>471</v>
+        <v>401</v>
       </c>
     </row>
     <row r="361" spans="1:3" outlineLevel="3">
       <c r="A361" s="8"/>
       <c r="B361" s="8"/>
       <c r="C361" s="9" t="s">
-        <v>472</v>
+        <v>402</v>
       </c>
     </row>
     <row r="362" spans="1:3" outlineLevel="3">
       <c r="A362" s="8"/>
       <c r="B362" s="8"/>
       <c r="C362" s="9" t="s">
-        <v>473</v>
+        <v>403</v>
       </c>
     </row>
     <row r="363" spans="1:3" outlineLevel="2">
@@ -4839,35 +4850,35 @@
       </c>
       <c r="B364" s="13"/>
       <c r="C364" s="12" t="s">
-        <v>474</v>
+        <v>404</v>
       </c>
     </row>
     <row r="365" spans="1:3" outlineLevel="3">
       <c r="A365" s="8"/>
       <c r="B365" s="8"/>
       <c r="C365" s="9" t="s">
-        <v>475</v>
+        <v>405</v>
       </c>
     </row>
     <row r="366" spans="1:3" outlineLevel="3">
       <c r="A366" s="8"/>
       <c r="B366" s="8"/>
       <c r="C366" s="9" t="s">
-        <v>476</v>
+        <v>406</v>
       </c>
     </row>
     <row r="367" spans="1:3" outlineLevel="3">
       <c r="A367" s="8"/>
       <c r="B367" s="8"/>
       <c r="C367" s="9" t="s">
-        <v>477</v>
+        <v>407</v>
       </c>
     </row>
     <row r="368" spans="1:3" outlineLevel="3">
       <c r="A368" s="8"/>
       <c r="B368" s="8"/>
       <c r="C368" s="9" t="s">
-        <v>478</v>
+        <v>408</v>
       </c>
     </row>
     <row r="369" spans="1:3" outlineLevel="2">
@@ -4881,35 +4892,35 @@
       </c>
       <c r="B370" s="13"/>
       <c r="C370" s="12" t="s">
-        <v>479</v>
+        <v>409</v>
       </c>
     </row>
     <row r="371" spans="1:3" outlineLevel="3">
       <c r="A371" s="8"/>
       <c r="B371" s="8"/>
       <c r="C371" s="9" t="s">
-        <v>480</v>
+        <v>410</v>
       </c>
     </row>
     <row r="372" spans="1:3" outlineLevel="3">
       <c r="A372" s="8"/>
       <c r="B372" s="8"/>
       <c r="C372" s="9" t="s">
-        <v>481</v>
+        <v>411</v>
       </c>
     </row>
     <row r="373" spans="1:3" outlineLevel="3">
       <c r="A373" s="8"/>
       <c r="B373" s="8"/>
       <c r="C373" s="9" t="s">
-        <v>482</v>
+        <v>412</v>
       </c>
     </row>
     <row r="374" spans="1:3" outlineLevel="3">
       <c r="A374" s="8"/>
       <c r="B374" s="8"/>
       <c r="C374" s="9" t="s">
-        <v>483</v>
+        <v>413</v>
       </c>
     </row>
     <row r="375" spans="1:3" outlineLevel="1">
@@ -4937,105 +4948,105 @@
       </c>
       <c r="B378" s="13"/>
       <c r="C378" s="12" t="s">
-        <v>484</v>
+        <v>414</v>
       </c>
     </row>
     <row r="379" spans="1:3" outlineLevel="3">
       <c r="A379" s="8"/>
       <c r="B379" s="8"/>
       <c r="C379" s="9" t="s">
-        <v>485</v>
+        <v>415</v>
       </c>
     </row>
     <row r="380" spans="1:3" outlineLevel="3">
       <c r="A380" s="8"/>
       <c r="B380" s="8"/>
       <c r="C380" s="9" t="s">
-        <v>486</v>
+        <v>416</v>
       </c>
     </row>
     <row r="381" spans="1:3" outlineLevel="3">
       <c r="A381" s="8"/>
       <c r="B381" s="8"/>
       <c r="C381" s="9" t="s">
-        <v>487</v>
+        <v>417</v>
       </c>
     </row>
     <row r="382" spans="1:3" outlineLevel="3">
       <c r="A382" s="8"/>
       <c r="B382" s="8"/>
       <c r="C382" s="9" t="s">
-        <v>488</v>
+        <v>418</v>
       </c>
     </row>
     <row r="383" spans="1:3" outlineLevel="3">
       <c r="A383" s="8"/>
       <c r="B383" s="8"/>
       <c r="C383" s="9" t="s">
-        <v>489</v>
+        <v>419</v>
       </c>
     </row>
     <row r="384" spans="1:3" outlineLevel="3">
       <c r="A384" s="8"/>
       <c r="B384" s="8"/>
       <c r="C384" s="9" t="s">
-        <v>490</v>
+        <v>420</v>
       </c>
     </row>
     <row r="385" spans="1:3" outlineLevel="3">
       <c r="A385" s="8"/>
       <c r="B385" s="8"/>
       <c r="C385" s="9" t="s">
-        <v>491</v>
+        <v>421</v>
       </c>
     </row>
     <row r="386" spans="1:3" outlineLevel="3">
       <c r="A386" s="8"/>
       <c r="B386" s="8"/>
       <c r="C386" s="9" t="s">
-        <v>492</v>
+        <v>422</v>
       </c>
     </row>
     <row r="387" spans="1:3" outlineLevel="3">
       <c r="A387" s="8"/>
       <c r="B387" s="8"/>
       <c r="C387" s="9" t="s">
-        <v>493</v>
+        <v>423</v>
       </c>
     </row>
     <row r="388" spans="1:3" outlineLevel="3">
       <c r="A388" s="8"/>
       <c r="B388" s="8"/>
       <c r="C388" s="9" t="s">
-        <v>494</v>
+        <v>424</v>
       </c>
     </row>
     <row r="389" spans="1:3" outlineLevel="3">
       <c r="A389" s="8"/>
       <c r="B389" s="8"/>
       <c r="C389" s="9" t="s">
-        <v>495</v>
+        <v>425</v>
       </c>
     </row>
     <row r="390" spans="1:3" outlineLevel="3">
       <c r="A390" s="8"/>
       <c r="B390" s="8"/>
       <c r="C390" s="9" t="s">
-        <v>496</v>
+        <v>426</v>
       </c>
     </row>
     <row r="391" spans="1:3" outlineLevel="3">
       <c r="A391" s="8"/>
       <c r="B391" s="8"/>
       <c r="C391" s="9" t="s">
-        <v>497</v>
+        <v>427</v>
       </c>
     </row>
     <row r="392" spans="1:3" outlineLevel="3">
       <c r="A392" s="8"/>
       <c r="B392" s="8"/>
       <c r="C392" s="9" t="s">
-        <v>498</v>
+        <v>428</v>
       </c>
     </row>
     <row r="393" spans="1:3" outlineLevel="2">
@@ -5049,49 +5060,49 @@
       </c>
       <c r="B394" s="13"/>
       <c r="C394" s="12" t="s">
-        <v>499</v>
+        <v>429</v>
       </c>
     </row>
     <row r="395" spans="1:3" outlineLevel="3">
       <c r="A395" s="8"/>
       <c r="B395" s="8"/>
       <c r="C395" s="9" t="s">
-        <v>500</v>
+        <v>430</v>
       </c>
     </row>
     <row r="396" spans="1:3" outlineLevel="3">
       <c r="A396" s="8"/>
       <c r="B396" s="8"/>
       <c r="C396" s="9" t="s">
-        <v>501</v>
+        <v>431</v>
       </c>
     </row>
     <row r="397" spans="1:3" outlineLevel="3">
       <c r="A397" s="8"/>
       <c r="B397" s="8"/>
       <c r="C397" s="9" t="s">
-        <v>502</v>
+        <v>432</v>
       </c>
     </row>
     <row r="398" spans="1:3" outlineLevel="3">
       <c r="A398" s="8"/>
       <c r="B398" s="8"/>
       <c r="C398" s="9" t="s">
-        <v>503</v>
+        <v>433</v>
       </c>
     </row>
     <row r="399" spans="1:3" outlineLevel="3">
       <c r="A399" s="8"/>
       <c r="B399" s="8"/>
       <c r="C399" s="9" t="s">
-        <v>504</v>
+        <v>434</v>
       </c>
     </row>
     <row r="400" spans="1:3" outlineLevel="3">
       <c r="A400" s="8"/>
       <c r="B400" s="8"/>
       <c r="C400" s="9" t="s">
-        <v>505</v>
+        <v>435</v>
       </c>
     </row>
     <row r="401" spans="1:3" outlineLevel="2">
@@ -5105,42 +5116,42 @@
       </c>
       <c r="B402" s="13"/>
       <c r="C402" s="12" t="s">
-        <v>506</v>
+        <v>436</v>
       </c>
     </row>
     <row r="403" spans="1:3" outlineLevel="3">
       <c r="A403" s="8"/>
       <c r="B403" s="8"/>
       <c r="C403" s="9" t="s">
-        <v>507</v>
+        <v>437</v>
       </c>
     </row>
     <row r="404" spans="1:3" outlineLevel="3">
       <c r="A404" s="8"/>
       <c r="B404" s="8"/>
       <c r="C404" s="9" t="s">
-        <v>508</v>
+        <v>438</v>
       </c>
     </row>
     <row r="405" spans="1:3" outlineLevel="3">
       <c r="A405" s="8"/>
       <c r="B405" s="8"/>
       <c r="C405" s="9" t="s">
-        <v>509</v>
+        <v>439</v>
       </c>
     </row>
     <row r="406" spans="1:3" outlineLevel="3">
       <c r="A406" s="8"/>
       <c r="B406" s="8"/>
       <c r="C406" s="9" t="s">
-        <v>510</v>
+        <v>440</v>
       </c>
     </row>
     <row r="407" spans="1:3" outlineLevel="3">
       <c r="A407" s="8"/>
       <c r="B407" s="8"/>
       <c r="C407" s="9" t="s">
-        <v>511</v>
+        <v>441</v>
       </c>
     </row>
     <row r="408" spans="1:3" outlineLevel="2">
@@ -5154,63 +5165,63 @@
       </c>
       <c r="B409" s="13"/>
       <c r="C409" s="12" t="s">
-        <v>512</v>
+        <v>442</v>
       </c>
     </row>
     <row r="410" spans="1:3" outlineLevel="3">
       <c r="A410" s="8"/>
       <c r="B410" s="8"/>
       <c r="C410" s="9" t="s">
-        <v>513</v>
+        <v>443</v>
       </c>
     </row>
     <row r="411" spans="1:3" outlineLevel="3">
       <c r="A411" s="8"/>
       <c r="B411" s="8"/>
       <c r="C411" s="9" t="s">
-        <v>514</v>
+        <v>444</v>
       </c>
     </row>
     <row r="412" spans="1:3" outlineLevel="3">
       <c r="A412" s="8"/>
       <c r="B412" s="8"/>
       <c r="C412" s="9" t="s">
-        <v>515</v>
+        <v>445</v>
       </c>
     </row>
     <row r="413" spans="1:3" outlineLevel="3">
       <c r="A413" s="8"/>
       <c r="B413" s="8"/>
       <c r="C413" s="9" t="s">
-        <v>516</v>
+        <v>446</v>
       </c>
     </row>
     <row r="414" spans="1:3" outlineLevel="3">
       <c r="A414" s="8"/>
       <c r="B414" s="8"/>
       <c r="C414" s="9" t="s">
-        <v>517</v>
+        <v>447</v>
       </c>
     </row>
     <row r="415" spans="1:3" outlineLevel="3">
       <c r="A415" s="8"/>
       <c r="B415" s="8"/>
       <c r="C415" s="9" t="s">
-        <v>518</v>
+        <v>448</v>
       </c>
     </row>
     <row r="416" spans="1:3" outlineLevel="3">
       <c r="A416" s="8"/>
       <c r="B416" s="8"/>
       <c r="C416" s="9" t="s">
-        <v>519</v>
+        <v>449</v>
       </c>
     </row>
     <row r="417" spans="1:3" outlineLevel="3">
       <c r="A417" s="8"/>
       <c r="B417" s="8"/>
       <c r="C417" s="9" t="s">
-        <v>520</v>
+        <v>450</v>
       </c>
     </row>
     <row r="418" spans="1:3" outlineLevel="1">
@@ -5238,70 +5249,70 @@
       </c>
       <c r="B421" s="13"/>
       <c r="C421" s="12" t="s">
-        <v>521</v>
+        <v>451</v>
       </c>
     </row>
     <row r="422" spans="1:3" outlineLevel="3">
       <c r="A422" s="8"/>
       <c r="B422" s="8"/>
       <c r="C422" s="9" t="s">
-        <v>522</v>
+        <v>452</v>
       </c>
     </row>
     <row r="423" spans="1:3" outlineLevel="3">
       <c r="A423" s="8"/>
       <c r="B423" s="8"/>
       <c r="C423" s="9" t="s">
-        <v>523</v>
+        <v>453</v>
       </c>
     </row>
     <row r="424" spans="1:3" outlineLevel="3">
       <c r="A424" s="8"/>
       <c r="B424" s="8"/>
       <c r="C424" s="9" t="s">
-        <v>524</v>
+        <v>454</v>
       </c>
     </row>
     <row r="425" spans="1:3" outlineLevel="3">
       <c r="A425" s="8"/>
       <c r="B425" s="8"/>
       <c r="C425" s="9" t="s">
-        <v>525</v>
+        <v>455</v>
       </c>
     </row>
     <row r="426" spans="1:3" outlineLevel="3">
       <c r="A426" s="8"/>
       <c r="B426" s="8"/>
       <c r="C426" s="9" t="s">
-        <v>526</v>
+        <v>456</v>
       </c>
     </row>
     <row r="427" spans="1:3" outlineLevel="3">
       <c r="A427" s="8"/>
       <c r="B427" s="8"/>
       <c r="C427" s="9" t="s">
-        <v>527</v>
+        <v>457</v>
       </c>
     </row>
     <row r="428" spans="1:3" outlineLevel="3">
       <c r="A428" s="8"/>
       <c r="B428" s="8"/>
       <c r="C428" s="9" t="s">
-        <v>528</v>
+        <v>458</v>
       </c>
     </row>
     <row r="429" spans="1:3" outlineLevel="3">
       <c r="A429" s="8"/>
       <c r="B429" s="8"/>
       <c r="C429" s="9" t="s">
-        <v>529</v>
+        <v>459</v>
       </c>
     </row>
     <row r="430" spans="1:3" outlineLevel="3">
       <c r="A430" s="8"/>
       <c r="B430" s="8"/>
       <c r="C430" s="9" t="s">
-        <v>530</v>
+        <v>460</v>
       </c>
     </row>
     <row r="431" spans="1:3" outlineLevel="2">
@@ -5315,28 +5326,28 @@
       </c>
       <c r="B432" s="13"/>
       <c r="C432" s="12" t="s">
-        <v>531</v>
+        <v>461</v>
       </c>
     </row>
     <row r="433" spans="1:3" outlineLevel="3">
       <c r="A433" s="8"/>
       <c r="B433" s="8"/>
       <c r="C433" s="9" t="s">
-        <v>532</v>
+        <v>462</v>
       </c>
     </row>
     <row r="434" spans="1:3" outlineLevel="3">
       <c r="A434" s="8"/>
       <c r="B434" s="8"/>
       <c r="C434" s="9" t="s">
-        <v>533</v>
+        <v>463</v>
       </c>
     </row>
     <row r="435" spans="1:3" outlineLevel="3">
       <c r="A435" s="8"/>
       <c r="B435" s="8"/>
       <c r="C435" s="9" t="s">
-        <v>534</v>
+        <v>464</v>
       </c>
     </row>
     <row r="436" spans="1:3" outlineLevel="2">
@@ -5350,35 +5361,35 @@
       </c>
       <c r="B437" s="13"/>
       <c r="C437" s="12" t="s">
-        <v>535</v>
+        <v>465</v>
       </c>
     </row>
     <row r="438" spans="1:3" outlineLevel="3">
       <c r="A438" s="8"/>
       <c r="B438" s="8"/>
       <c r="C438" s="9" t="s">
-        <v>536</v>
+        <v>466</v>
       </c>
     </row>
     <row r="439" spans="1:3" outlineLevel="3">
       <c r="A439" s="8"/>
       <c r="B439" s="8"/>
       <c r="C439" s="9" t="s">
-        <v>537</v>
+        <v>467</v>
       </c>
     </row>
     <row r="440" spans="1:3" outlineLevel="3">
       <c r="A440" s="8"/>
       <c r="B440" s="8"/>
       <c r="C440" s="9" t="s">
-        <v>538</v>
+        <v>468</v>
       </c>
     </row>
     <row r="441" spans="1:3" outlineLevel="3">
       <c r="A441" s="8"/>
       <c r="B441" s="8"/>
       <c r="C441" s="9" t="s">
-        <v>539</v>
+        <v>469</v>
       </c>
     </row>
     <row r="442" spans="1:3" outlineLevel="2">
@@ -5392,42 +5403,42 @@
       </c>
       <c r="B443" s="13"/>
       <c r="C443" s="12" t="s">
-        <v>540</v>
+        <v>470</v>
       </c>
     </row>
     <row r="444" spans="1:3" outlineLevel="3">
       <c r="A444" s="8"/>
       <c r="B444" s="8"/>
       <c r="C444" s="9" t="s">
-        <v>541</v>
+        <v>471</v>
       </c>
     </row>
     <row r="445" spans="1:3" outlineLevel="3">
       <c r="A445" s="8"/>
       <c r="B445" s="8"/>
       <c r="C445" s="9" t="s">
-        <v>542</v>
+        <v>472</v>
       </c>
     </row>
     <row r="446" spans="1:3" outlineLevel="3">
       <c r="A446" s="8"/>
       <c r="B446" s="8"/>
       <c r="C446" s="9" t="s">
-        <v>543</v>
+        <v>473</v>
       </c>
     </row>
     <row r="447" spans="1:3" outlineLevel="3">
       <c r="A447" s="8"/>
       <c r="B447" s="8"/>
       <c r="C447" s="9" t="s">
-        <v>544</v>
+        <v>474</v>
       </c>
     </row>
     <row r="448" spans="1:3" outlineLevel="3">
       <c r="A448" s="8"/>
       <c r="B448" s="8"/>
       <c r="C448" s="9" t="s">
-        <v>545</v>
+        <v>475</v>
       </c>
     </row>
     <row r="449" spans="1:3" outlineLevel="2">
@@ -5437,46 +5448,46 @@
     </row>
     <row r="450" spans="1:3" outlineLevel="2">
       <c r="A450" s="12" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="B450" s="13"/>
       <c r="C450" s="12" t="s">
-        <v>546</v>
+        <v>476</v>
       </c>
     </row>
     <row r="451" spans="1:3" outlineLevel="3">
       <c r="A451" s="8"/>
       <c r="B451" s="8"/>
       <c r="C451" s="9" t="s">
-        <v>547</v>
+        <v>477</v>
       </c>
     </row>
     <row r="452" spans="1:3" outlineLevel="3">
       <c r="A452" s="8"/>
       <c r="B452" s="8"/>
       <c r="C452" s="9" t="s">
-        <v>548</v>
+        <v>478</v>
       </c>
     </row>
     <row r="453" spans="1:3" outlineLevel="3">
       <c r="A453" s="8"/>
       <c r="B453" s="8"/>
       <c r="C453" s="9" t="s">
-        <v>549</v>
+        <v>479</v>
       </c>
     </row>
     <row r="454" spans="1:3" outlineLevel="3">
       <c r="A454" s="8"/>
       <c r="B454" s="8"/>
       <c r="C454" s="9" t="s">
-        <v>550</v>
+        <v>480</v>
       </c>
     </row>
     <row r="455" spans="1:3" outlineLevel="3">
       <c r="A455" s="8"/>
       <c r="B455" s="8"/>
       <c r="C455" s="9" t="s">
-        <v>551</v>
+        <v>481</v>
       </c>
     </row>
     <row r="456" spans="1:3" outlineLevel="2">
@@ -5486,88 +5497,88 @@
     </row>
     <row r="457" spans="1:3" outlineLevel="2">
       <c r="A457" s="12" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B457" s="13"/>
       <c r="C457" s="12" t="s">
-        <v>552</v>
+        <v>482</v>
       </c>
     </row>
     <row r="458" spans="1:3" outlineLevel="3">
       <c r="A458" s="8"/>
       <c r="B458" s="8"/>
       <c r="C458" s="9" t="s">
-        <v>553</v>
+        <v>483</v>
       </c>
     </row>
     <row r="459" spans="1:3" outlineLevel="3">
       <c r="A459" s="8"/>
       <c r="B459" s="8"/>
       <c r="C459" s="9" t="s">
-        <v>554</v>
+        <v>484</v>
       </c>
     </row>
     <row r="460" spans="1:3" outlineLevel="3">
       <c r="A460" s="8"/>
       <c r="B460" s="8"/>
       <c r="C460" s="9" t="s">
-        <v>555</v>
+        <v>485</v>
       </c>
     </row>
     <row r="461" spans="1:3" outlineLevel="3">
       <c r="A461" s="8"/>
       <c r="B461" s="8"/>
       <c r="C461" s="9" t="s">
-        <v>556</v>
+        <v>486</v>
       </c>
     </row>
     <row r="462" spans="1:3" outlineLevel="3">
       <c r="A462" s="8"/>
       <c r="B462" s="8"/>
       <c r="C462" s="9" t="s">
-        <v>557</v>
+        <v>487</v>
       </c>
     </row>
     <row r="463" spans="1:3" outlineLevel="3">
       <c r="A463" s="8"/>
       <c r="B463" s="8"/>
       <c r="C463" s="9" t="s">
-        <v>558</v>
+        <v>488</v>
       </c>
     </row>
     <row r="464" spans="1:3" outlineLevel="3">
       <c r="A464" s="8"/>
       <c r="B464" s="8"/>
       <c r="C464" s="9" t="s">
-        <v>559</v>
+        <v>489</v>
       </c>
     </row>
     <row r="465" spans="1:3" outlineLevel="3">
       <c r="A465" s="8"/>
       <c r="B465" s="8"/>
       <c r="C465" s="9" t="s">
-        <v>560</v>
+        <v>490</v>
       </c>
     </row>
     <row r="466" spans="1:3" outlineLevel="3">
       <c r="A466" s="8"/>
       <c r="B466" s="8"/>
       <c r="C466" s="9" t="s">
-        <v>561</v>
+        <v>491</v>
       </c>
     </row>
     <row r="467" spans="1:3" outlineLevel="3">
       <c r="A467" s="8"/>
       <c r="B467" s="8"/>
       <c r="C467" s="9" t="s">
-        <v>562</v>
+        <v>492</v>
       </c>
     </row>
     <row r="468" spans="1:3" outlineLevel="3">
       <c r="A468" s="8"/>
       <c r="B468" s="8"/>
       <c r="C468" s="9" t="s">
-        <v>563</v>
+        <v>493</v>
       </c>
     </row>
     <row r="469" spans="1:3" outlineLevel="1">
@@ -5577,11 +5588,11 @@
     </row>
     <row r="470" spans="1:3" outlineLevel="1">
       <c r="A470" s="7" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B470" s="7"/>
       <c r="C470" s="7" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="471" spans="1:3" outlineLevel="2">
@@ -5591,53 +5602,53 @@
     </row>
     <row r="472" spans="1:3" outlineLevel="2">
       <c r="A472" s="12" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="B472" s="13"/>
       <c r="C472" s="12" t="s">
-        <v>129</v>
+        <v>494</v>
       </c>
     </row>
     <row r="473" spans="1:3" outlineLevel="3">
       <c r="A473" s="8"/>
       <c r="B473" s="8"/>
       <c r="C473" s="9" t="s">
-        <v>130</v>
+        <v>495</v>
       </c>
     </row>
     <row r="474" spans="1:3" outlineLevel="3">
       <c r="A474" s="8"/>
       <c r="B474" s="8"/>
       <c r="C474" s="9" t="s">
-        <v>131</v>
+        <v>496</v>
       </c>
     </row>
     <row r="475" spans="1:3" outlineLevel="3">
       <c r="A475" s="8"/>
       <c r="B475" s="8"/>
-      <c r="C475" s="9" t="s">
-        <v>132</v>
+      <c r="C475" s="16" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="476" spans="1:3" outlineLevel="3">
       <c r="A476" s="8"/>
       <c r="B476" s="8"/>
       <c r="C476" s="9" t="s">
-        <v>133</v>
+        <v>498</v>
       </c>
     </row>
     <row r="477" spans="1:3" outlineLevel="3">
       <c r="A477" s="8"/>
       <c r="B477" s="8"/>
       <c r="C477" s="9" t="s">
-        <v>104</v>
+        <v>499</v>
       </c>
     </row>
     <row r="478" spans="1:3" outlineLevel="3">
       <c r="A478" s="8"/>
       <c r="B478" s="8"/>
       <c r="C478" s="9" t="s">
-        <v>105</v>
+        <v>500</v>
       </c>
     </row>
     <row r="479" spans="1:3" outlineLevel="2">
@@ -5647,32 +5658,32 @@
     </row>
     <row r="480" spans="1:3" outlineLevel="2">
       <c r="A480" s="12" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="B480" s="13"/>
       <c r="C480" s="12" t="s">
-        <v>134</v>
+        <v>501</v>
       </c>
     </row>
     <row r="481" spans="1:3" outlineLevel="3">
       <c r="A481" s="8"/>
       <c r="B481" s="8"/>
       <c r="C481" s="9" t="s">
-        <v>106</v>
+        <v>502</v>
       </c>
     </row>
     <row r="482" spans="1:3" outlineLevel="3">
       <c r="A482" s="8"/>
       <c r="B482" s="8"/>
       <c r="C482" s="9" t="s">
-        <v>107</v>
+        <v>503</v>
       </c>
     </row>
     <row r="483" spans="1:3" outlineLevel="3">
       <c r="A483" s="8"/>
       <c r="B483" s="8"/>
       <c r="C483" s="9" t="s">
-        <v>108</v>
+        <v>504</v>
       </c>
     </row>
     <row r="484" spans="1:3" outlineLevel="2">
@@ -5682,46 +5693,46 @@
     </row>
     <row r="485" spans="1:3" outlineLevel="2">
       <c r="A485" s="12" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B485" s="13"/>
       <c r="C485" s="12" t="s">
-        <v>141</v>
+        <v>505</v>
       </c>
     </row>
     <row r="486" spans="1:3" outlineLevel="3">
       <c r="A486" s="8"/>
       <c r="B486" s="8"/>
       <c r="C486" s="9" t="s">
-        <v>109</v>
+        <v>506</v>
       </c>
     </row>
     <row r="487" spans="1:3" outlineLevel="3">
       <c r="A487" s="8"/>
       <c r="B487" s="8"/>
       <c r="C487" s="9" t="s">
-        <v>135</v>
+        <v>507</v>
       </c>
     </row>
     <row r="488" spans="1:3" outlineLevel="3">
       <c r="A488" s="8"/>
       <c r="B488" s="8"/>
       <c r="C488" s="9" t="s">
-        <v>136</v>
+        <v>508</v>
       </c>
     </row>
     <row r="489" spans="1:3" outlineLevel="3">
       <c r="A489" s="8"/>
       <c r="B489" s="8"/>
       <c r="C489" s="9" t="s">
-        <v>110</v>
+        <v>509</v>
       </c>
     </row>
     <row r="490" spans="1:3" outlineLevel="3">
       <c r="A490" s="8"/>
       <c r="B490" s="8"/>
       <c r="C490" s="9" t="s">
-        <v>111</v>
+        <v>510</v>
       </c>
     </row>
     <row r="491" spans="1:3" outlineLevel="2">
@@ -5731,32 +5742,32 @@
     </row>
     <row r="492" spans="1:3" outlineLevel="2">
       <c r="A492" s="12" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="B492" s="13"/>
       <c r="C492" s="12" t="s">
-        <v>142</v>
+        <v>511</v>
       </c>
     </row>
     <row r="493" spans="1:3" outlineLevel="3">
       <c r="A493" s="8"/>
       <c r="B493" s="8"/>
       <c r="C493" s="9" t="s">
-        <v>112</v>
+        <v>513</v>
       </c>
     </row>
     <row r="494" spans="1:3" outlineLevel="3">
       <c r="A494" s="8"/>
       <c r="B494" s="8"/>
       <c r="C494" s="9" t="s">
-        <v>113</v>
+        <v>512</v>
       </c>
     </row>
     <row r="495" spans="1:3" outlineLevel="3">
       <c r="A495" s="8"/>
       <c r="B495" s="8"/>
       <c r="C495" s="9" t="s">
-        <v>114</v>
+        <v>514</v>
       </c>
     </row>
     <row r="496" spans="1:3" outlineLevel="2">
@@ -5766,39 +5777,39 @@
     </row>
     <row r="497" spans="1:3" outlineLevel="2">
       <c r="A497" s="12" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="B497" s="13"/>
       <c r="C497" s="12" t="s">
-        <v>143</v>
+        <v>515</v>
       </c>
     </row>
     <row r="498" spans="1:3" outlineLevel="3">
       <c r="A498" s="8"/>
       <c r="B498" s="8"/>
       <c r="C498" s="9" t="s">
-        <v>137</v>
+        <v>516</v>
       </c>
     </row>
     <row r="499" spans="1:3" outlineLevel="3">
       <c r="A499" s="8"/>
       <c r="B499" s="8"/>
       <c r="C499" s="9" t="s">
-        <v>138</v>
+        <v>517</v>
       </c>
     </row>
     <row r="500" spans="1:3" outlineLevel="3">
       <c r="A500" s="8"/>
       <c r="B500" s="8"/>
       <c r="C500" s="9" t="s">
-        <v>115</v>
+        <v>518</v>
       </c>
     </row>
     <row r="501" spans="1:3" outlineLevel="3">
       <c r="A501" s="8"/>
       <c r="B501" s="8"/>
       <c r="C501" s="9" t="s">
-        <v>116</v>
+        <v>519</v>
       </c>
     </row>
     <row r="502" spans="1:3" outlineLevel="2">
@@ -5808,67 +5819,67 @@
     </row>
     <row r="503" spans="1:3" outlineLevel="2">
       <c r="A503" s="12" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="B503" s="13"/>
       <c r="C503" s="12" t="s">
-        <v>144</v>
+        <v>520</v>
       </c>
     </row>
     <row r="504" spans="1:3" outlineLevel="3">
       <c r="A504" s="8"/>
       <c r="B504" s="8"/>
-      <c r="C504" s="9" t="s">
-        <v>140</v>
+      <c r="C504" s="16" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="505" spans="1:3" outlineLevel="3">
       <c r="A505" s="8"/>
       <c r="B505" s="8"/>
       <c r="C505" s="9" t="s">
-        <v>139</v>
+        <v>521</v>
       </c>
     </row>
     <row r="506" spans="1:3" outlineLevel="3">
       <c r="A506" s="8"/>
       <c r="B506" s="8"/>
       <c r="C506" s="9" t="s">
-        <v>117</v>
+        <v>522</v>
       </c>
     </row>
     <row r="507" spans="1:3" outlineLevel="3">
       <c r="A507" s="8"/>
       <c r="B507" s="8"/>
       <c r="C507" s="9" t="s">
-        <v>118</v>
+        <v>523</v>
       </c>
     </row>
     <row r="508" spans="1:3" outlineLevel="3">
       <c r="A508" s="8"/>
       <c r="B508" s="8"/>
       <c r="C508" s="9" t="s">
-        <v>145</v>
+        <v>524</v>
       </c>
     </row>
     <row r="509" spans="1:3" outlineLevel="3">
       <c r="A509" s="8"/>
       <c r="B509" s="8"/>
       <c r="C509" s="9" t="s">
-        <v>146</v>
+        <v>525</v>
       </c>
     </row>
     <row r="510" spans="1:3" outlineLevel="3">
       <c r="A510" s="8"/>
       <c r="B510" s="8"/>
       <c r="C510" s="9" t="s">
-        <v>147</v>
+        <v>526</v>
       </c>
     </row>
     <row r="511" spans="1:3" outlineLevel="3">
       <c r="A511" s="8"/>
       <c r="B511" s="8"/>
       <c r="C511" s="9" t="s">
-        <v>148</v>
+        <v>527</v>
       </c>
     </row>
     <row r="512" spans="1:3" outlineLevel="1">
@@ -5878,11 +5889,11 @@
     </row>
     <row r="513" spans="1:3" outlineLevel="1">
       <c r="A513" s="7" t="s">
-        <v>171</v>
+        <v>115</v>
       </c>
       <c r="B513" s="7"/>
       <c r="C513" s="7" t="s">
-        <v>178</v>
+        <v>122</v>
       </c>
     </row>
     <row r="514" spans="1:3" outlineLevel="2">
@@ -5892,39 +5903,39 @@
     </row>
     <row r="515" spans="1:3" outlineLevel="2">
       <c r="A515" s="12" t="s">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="B515" s="13"/>
       <c r="C515" s="12" t="s">
-        <v>179</v>
+        <v>528</v>
       </c>
     </row>
     <row r="516" spans="1:3" outlineLevel="3">
       <c r="A516" s="8"/>
       <c r="B516" s="8"/>
       <c r="C516" s="9" t="s">
-        <v>149</v>
+        <v>529</v>
       </c>
     </row>
     <row r="517" spans="1:3" outlineLevel="3">
       <c r="A517" s="8"/>
       <c r="B517" s="8"/>
       <c r="C517" s="9" t="s">
-        <v>150</v>
+        <v>530</v>
       </c>
     </row>
     <row r="518" spans="1:3" outlineLevel="3">
       <c r="A518" s="8"/>
       <c r="B518" s="8"/>
       <c r="C518" s="9" t="s">
-        <v>151</v>
+        <v>531</v>
       </c>
     </row>
     <row r="519" spans="1:3" outlineLevel="3">
       <c r="A519" s="8"/>
       <c r="B519" s="8"/>
       <c r="C519" s="9" t="s">
-        <v>152</v>
+        <v>532</v>
       </c>
     </row>
     <row r="520" spans="1:3" outlineLevel="2">
@@ -5934,60 +5945,60 @@
     </row>
     <row r="521" spans="1:3" outlineLevel="2">
       <c r="A521" s="12" t="s">
-        <v>173</v>
+        <v>117</v>
       </c>
       <c r="B521" s="13"/>
       <c r="C521" s="12" t="s">
-        <v>184</v>
+        <v>533</v>
       </c>
     </row>
     <row r="522" spans="1:3" outlineLevel="3">
       <c r="A522" s="8"/>
       <c r="B522" s="8"/>
       <c r="C522" s="9" t="s">
-        <v>180</v>
+        <v>534</v>
       </c>
     </row>
     <row r="523" spans="1:3" outlineLevel="3">
       <c r="A523" s="8"/>
       <c r="B523" s="8"/>
       <c r="C523" s="9" t="s">
-        <v>181</v>
+        <v>535</v>
       </c>
     </row>
     <row r="524" spans="1:3" outlineLevel="3">
       <c r="A524" s="8"/>
       <c r="B524" s="8"/>
       <c r="C524" s="9" t="s">
-        <v>153</v>
+        <v>536</v>
       </c>
     </row>
     <row r="525" spans="1:3" outlineLevel="3">
       <c r="A525" s="8"/>
       <c r="B525" s="8"/>
       <c r="C525" s="9" t="s">
-        <v>154</v>
+        <v>537</v>
       </c>
     </row>
     <row r="526" spans="1:3" outlineLevel="3">
       <c r="A526" s="8"/>
       <c r="B526" s="8"/>
       <c r="C526" s="9" t="s">
-        <v>182</v>
+        <v>538</v>
       </c>
     </row>
     <row r="527" spans="1:3" outlineLevel="3">
       <c r="A527" s="8"/>
       <c r="B527" s="8"/>
       <c r="C527" s="9" t="s">
-        <v>183</v>
+        <v>539</v>
       </c>
     </row>
     <row r="528" spans="1:3" outlineLevel="3">
       <c r="A528" s="8"/>
       <c r="B528" s="8"/>
       <c r="C528" s="9" t="s">
-        <v>155</v>
+        <v>540</v>
       </c>
     </row>
     <row r="529" spans="1:3" outlineLevel="2">
@@ -5997,39 +6008,39 @@
     </row>
     <row r="530" spans="1:3" outlineLevel="2">
       <c r="A530" s="12" t="s">
-        <v>174</v>
+        <v>118</v>
       </c>
       <c r="B530" s="13"/>
       <c r="C530" s="12" t="s">
-        <v>185</v>
+        <v>541</v>
       </c>
     </row>
     <row r="531" spans="1:3" outlineLevel="3">
       <c r="A531" s="8"/>
       <c r="B531" s="8"/>
       <c r="C531" s="9" t="s">
-        <v>156</v>
+        <v>542</v>
       </c>
     </row>
     <row r="532" spans="1:3" outlineLevel="3">
       <c r="A532" s="8"/>
       <c r="B532" s="8"/>
       <c r="C532" s="9" t="s">
-        <v>157</v>
+        <v>543</v>
       </c>
     </row>
     <row r="533" spans="1:3" outlineLevel="3">
       <c r="A533" s="8"/>
       <c r="B533" s="8"/>
       <c r="C533" s="9" t="s">
-        <v>158</v>
+        <v>544</v>
       </c>
     </row>
     <row r="534" spans="1:3" outlineLevel="3">
       <c r="A534" s="8"/>
       <c r="B534" s="8"/>
       <c r="C534" s="9" t="s">
-        <v>159</v>
+        <v>545</v>
       </c>
     </row>
     <row r="535" spans="1:3" outlineLevel="2">
@@ -6039,39 +6050,39 @@
     </row>
     <row r="536" spans="1:3" outlineLevel="2">
       <c r="A536" s="12" t="s">
-        <v>175</v>
+        <v>119</v>
       </c>
       <c r="B536" s="13"/>
       <c r="C536" s="12" t="s">
-        <v>186</v>
+        <v>546</v>
       </c>
     </row>
     <row r="537" spans="1:3" outlineLevel="3">
       <c r="A537" s="8"/>
       <c r="B537" s="8"/>
       <c r="C537" s="9" t="s">
-        <v>160</v>
+        <v>547</v>
       </c>
     </row>
     <row r="538" spans="1:3" outlineLevel="3">
       <c r="A538" s="8"/>
       <c r="B538" s="8"/>
       <c r="C538" s="9" t="s">
-        <v>161</v>
+        <v>548</v>
       </c>
     </row>
     <row r="539" spans="1:3" outlineLevel="3">
       <c r="A539" s="8"/>
       <c r="B539" s="8"/>
       <c r="C539" s="9" t="s">
-        <v>162</v>
+        <v>549</v>
       </c>
     </row>
     <row r="540" spans="1:3" outlineLevel="3">
       <c r="A540" s="8"/>
       <c r="B540" s="8"/>
       <c r="C540" s="9" t="s">
-        <v>163</v>
+        <v>550</v>
       </c>
     </row>
     <row r="541" spans="1:3" outlineLevel="2">
@@ -6081,39 +6092,39 @@
     </row>
     <row r="542" spans="1:3" outlineLevel="2">
       <c r="A542" s="12" t="s">
-        <v>176</v>
+        <v>120</v>
       </c>
       <c r="B542" s="13"/>
-      <c r="C542" s="12" t="s">
-        <v>187</v>
+      <c r="C542" s="17" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="543" spans="1:3" outlineLevel="3">
       <c r="A543" s="8"/>
       <c r="B543" s="8"/>
       <c r="C543" s="9" t="s">
-        <v>164</v>
+        <v>552</v>
       </c>
     </row>
     <row r="544" spans="1:3" outlineLevel="3">
       <c r="A544" s="8"/>
       <c r="B544" s="8"/>
       <c r="C544" s="9" t="s">
-        <v>165</v>
+        <v>553</v>
       </c>
     </row>
     <row r="545" spans="1:3" outlineLevel="3">
       <c r="A545" s="8"/>
       <c r="B545" s="8"/>
-      <c r="C545" s="9" t="s">
-        <v>166</v>
+      <c r="C545" s="16" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="546" spans="1:3" outlineLevel="3">
       <c r="A546" s="8"/>
       <c r="B546" s="8"/>
       <c r="C546" s="9" t="s">
-        <v>167</v>
+        <v>555</v>
       </c>
     </row>
     <row r="547" spans="1:3" outlineLevel="2">
@@ -6123,67 +6134,67 @@
     </row>
     <row r="548" spans="1:3" outlineLevel="2">
       <c r="A548" s="12" t="s">
-        <v>177</v>
+        <v>121</v>
       </c>
       <c r="B548" s="13"/>
       <c r="C548" s="12" t="s">
-        <v>188</v>
+        <v>556</v>
       </c>
     </row>
     <row r="549" spans="1:3" outlineLevel="3">
       <c r="A549" s="8"/>
       <c r="B549" s="8"/>
       <c r="C549" s="9" t="s">
-        <v>189</v>
+        <v>557</v>
       </c>
     </row>
     <row r="550" spans="1:3" outlineLevel="3">
       <c r="A550" s="8"/>
       <c r="B550" s="8"/>
       <c r="C550" s="9" t="s">
-        <v>190</v>
+        <v>558</v>
       </c>
     </row>
     <row r="551" spans="1:3" outlineLevel="3">
       <c r="A551" s="8"/>
       <c r="B551" s="8"/>
       <c r="C551" s="9" t="s">
-        <v>191</v>
+        <v>559</v>
       </c>
     </row>
     <row r="552" spans="1:3" outlineLevel="3">
       <c r="A552" s="8"/>
       <c r="B552" s="8"/>
       <c r="C552" s="9" t="s">
-        <v>192</v>
+        <v>560</v>
       </c>
     </row>
     <row r="553" spans="1:3" outlineLevel="3">
       <c r="A553" s="8"/>
       <c r="B553" s="8"/>
       <c r="C553" s="9" t="s">
-        <v>168</v>
+        <v>561</v>
       </c>
     </row>
     <row r="554" spans="1:3" outlineLevel="3">
       <c r="A554" s="8"/>
       <c r="B554" s="8"/>
       <c r="C554" s="9" t="s">
-        <v>169</v>
+        <v>562</v>
       </c>
     </row>
     <row r="555" spans="1:3" outlineLevel="3">
       <c r="A555" s="8"/>
       <c r="B555" s="8"/>
       <c r="C555" s="9" t="s">
-        <v>146</v>
+        <v>563</v>
       </c>
     </row>
     <row r="556" spans="1:3" outlineLevel="3">
       <c r="A556" s="8"/>
       <c r="B556" s="8"/>
       <c r="C556" s="9" t="s">
-        <v>170</v>
+        <v>564</v>
       </c>
     </row>
     <row r="557" spans="1:3" ht="16" thickBot="1">

</xml_diff>

<commit_message>
Insert Topic and Subtopic Scripts
</commit_message>
<xml_diff>
--- a/SPREADSHEETS/Survey Form-Spanish.xlsx
+++ b/SPREADSHEETS/Survey Form-Spanish.xlsx
@@ -366,9 +366,6 @@
     <t>IMPLEMENTING</t>
   </si>
   <si>
-    <t>Sourcing and partnering</t>
-  </si>
-  <si>
     <t>4.6.0</t>
   </si>
   <si>
@@ -1515,9 +1512,6 @@
     <t>El diseño del sistema de implementacion:</t>
   </si>
   <si>
-    <t>Asignacion de tareas y cell/unit layout</t>
-  </si>
-  <si>
     <t>Flujo de trabajo</t>
   </si>
   <si>
@@ -1677,18 +1671,12 @@
     <t>Soluciones/Mejoras de contingencia resultantes de la necesidad operacional</t>
   </si>
   <si>
-    <t>Cuestiones relativas a la Eliminacion y Life-End (Disposal and Life-End Issues)</t>
-  </si>
-  <si>
     <t>La terminacion de la vida util</t>
   </si>
   <si>
     <t>Opciones de eliminacion</t>
   </si>
   <si>
-    <t>Valor residual al life-end</t>
-  </si>
-  <si>
     <t>Consideraciones ambientales para la eliminacion</t>
   </si>
   <si>
@@ -1717,6 +1705,18 @@
   </si>
   <si>
     <t>Seguridad Ambiental</t>
+  </si>
+  <si>
+    <t>Asignacion y disposicion de tareas</t>
+  </si>
+  <si>
+    <t>Abastecimiento y Asociaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuestiones relativas a la Eliminacion y al Fin del Ciclo de Vida </t>
+  </si>
+  <si>
+    <t>Valor residual al fin del ciclo de vida</t>
   </si>
 </sst>
 </file>
@@ -1780,7 +1780,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1813,12 +1813,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1878,7 +1872,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1888,8 +1882,80 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1912,16 +1978,86 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="81">
     <cellStyle name="Buena 2" xfId="6"/>
     <cellStyle name="Comma 2" xfId="4"/>
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Percent 2" xfId="5"/>
@@ -2271,8 +2407,8 @@
   </sheetPr>
   <dimension ref="A1:G557"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A532" workbookViewId="0">
-      <selection activeCell="C557" sqref="C557"/>
+    <sheetView tabSelected="1" topLeftCell="A523" workbookViewId="0">
+      <selection activeCell="C553" sqref="C553"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="3" x14ac:dyDescent="0"/>
@@ -2329,7 +2465,7 @@
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>0</v>
@@ -2339,7 +2475,7 @@
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>1</v>
@@ -2349,7 +2485,7 @@
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>2</v>
@@ -2359,7 +2495,7 @@
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>3</v>
@@ -2369,7 +2505,7 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>4</v>
@@ -2386,21 +2522,21 @@
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:7" outlineLevel="3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:7" outlineLevel="3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:7" outlineLevel="2">
@@ -2414,21 +2550,21 @@
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:3" outlineLevel="3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:3" outlineLevel="3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:3" outlineLevel="2">
@@ -2442,35 +2578,35 @@
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:3" outlineLevel="3">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:3" outlineLevel="3">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:3" outlineLevel="3">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:3" outlineLevel="3">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:3" outlineLevel="2">
@@ -2484,35 +2620,35 @@
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:3" outlineLevel="3">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:3" outlineLevel="3">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:3" outlineLevel="3">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:3" outlineLevel="3">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:3" outlineLevel="1">
@@ -2540,21 +2676,21 @@
       </c>
       <c r="B34" s="13"/>
       <c r="C34" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:3" outlineLevel="3">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:3" outlineLevel="3">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:3" outlineLevel="2">
@@ -2568,49 +2704,49 @@
       </c>
       <c r="B38" s="13"/>
       <c r="C38" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:3" outlineLevel="3">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:3" outlineLevel="3">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:3" outlineLevel="3">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:3" outlineLevel="3">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:3" outlineLevel="3">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:3" outlineLevel="3">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:3" outlineLevel="2">
@@ -2624,42 +2760,42 @@
       </c>
       <c r="B46" s="13"/>
       <c r="C46" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:3" outlineLevel="3">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:3" outlineLevel="3">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:3" outlineLevel="3">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:3" outlineLevel="3">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:3" outlineLevel="3">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52" spans="1:3" outlineLevel="2">
@@ -2673,28 +2809,28 @@
       </c>
       <c r="B53" s="13"/>
       <c r="C53" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:3" outlineLevel="3">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:3" outlineLevel="3">
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" spans="1:3" outlineLevel="3">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:3" outlineLevel="1">
@@ -2722,35 +2858,35 @@
       </c>
       <c r="B60" s="13"/>
       <c r="C60" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:3" outlineLevel="3">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="62" spans="1:3" outlineLevel="3">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="C62" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:3" outlineLevel="3">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="64" spans="1:3" outlineLevel="3">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="65" spans="1:3" outlineLevel="2">
@@ -2764,35 +2900,35 @@
       </c>
       <c r="B66" s="13"/>
       <c r="C66" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="67" spans="1:3" outlineLevel="3">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:3" outlineLevel="3">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:3" outlineLevel="3">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="70" spans="1:3" outlineLevel="3">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:3" outlineLevel="2">
@@ -2806,28 +2942,28 @@
       </c>
       <c r="B72" s="13"/>
       <c r="C72" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="73" spans="1:3" outlineLevel="3">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="74" spans="1:3" outlineLevel="3">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:3" outlineLevel="3">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="76" spans="1:3" outlineLevel="2">
@@ -2841,28 +2977,28 @@
       </c>
       <c r="B77" s="13"/>
       <c r="C77" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="78" spans="1:3" outlineLevel="3">
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:3" outlineLevel="3">
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="C79" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:3" outlineLevel="3">
       <c r="A80" s="8"/>
       <c r="B80" s="8"/>
       <c r="C80" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="81" spans="1:3" outlineLevel="1">
@@ -2890,35 +3026,35 @@
       </c>
       <c r="B84" s="13"/>
       <c r="C84" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="85" spans="1:3" outlineLevel="3">
       <c r="A85" s="8"/>
       <c r="B85" s="8"/>
       <c r="C85" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="86" spans="1:3" outlineLevel="3">
       <c r="A86" s="8"/>
       <c r="B86" s="8"/>
       <c r="C86" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="87" spans="1:3" outlineLevel="3">
       <c r="A87" s="8"/>
       <c r="B87" s="8"/>
       <c r="C87" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="88" spans="1:3" outlineLevel="3">
       <c r="A88" s="8"/>
       <c r="B88" s="8"/>
       <c r="C88" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="89" spans="1:3" outlineLevel="2">
@@ -2932,70 +3068,70 @@
       </c>
       <c r="B90" s="13"/>
       <c r="C90" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="91" spans="1:3" outlineLevel="3">
       <c r="A91" s="8"/>
       <c r="B91" s="8"/>
       <c r="C91" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="92" spans="1:3" outlineLevel="3">
       <c r="A92" s="8"/>
       <c r="B92" s="8"/>
       <c r="C92" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="93" spans="1:3" outlineLevel="3">
       <c r="A93" s="8"/>
       <c r="B93" s="8"/>
       <c r="C93" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="94" spans="1:3" outlineLevel="3">
       <c r="A94" s="8"/>
       <c r="B94" s="8"/>
       <c r="C94" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="95" spans="1:3" outlineLevel="3">
       <c r="A95" s="8"/>
       <c r="B95" s="8"/>
       <c r="C95" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="96" spans="1:3" outlineLevel="3">
       <c r="A96" s="8"/>
       <c r="B96" s="8"/>
       <c r="C96" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="97" spans="1:3" outlineLevel="3">
       <c r="A97" s="8"/>
       <c r="B97" s="8"/>
       <c r="C97" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="98" spans="1:3" outlineLevel="3">
       <c r="A98" s="8"/>
       <c r="B98" s="8"/>
       <c r="C98" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="99" spans="1:3" outlineLevel="3">
       <c r="A99" s="8"/>
       <c r="B99" s="8"/>
       <c r="C99" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="100" spans="1:3" outlineLevel="2">
@@ -3009,35 +3145,35 @@
       </c>
       <c r="B101" s="13"/>
       <c r="C101" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="102" spans="1:3" outlineLevel="3">
       <c r="A102" s="8"/>
       <c r="B102" s="8"/>
       <c r="C102" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="103" spans="1:3" outlineLevel="3">
       <c r="A103" s="8"/>
       <c r="B103" s="8"/>
       <c r="C103" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="104" spans="1:3" outlineLevel="3">
       <c r="A104" s="8"/>
       <c r="B104" s="8"/>
       <c r="C104" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="105" spans="1:3" outlineLevel="3">
       <c r="A105" s="8"/>
       <c r="B105" s="8"/>
       <c r="C105" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="106" spans="1:3" outlineLevel="2">
@@ -3051,49 +3187,49 @@
       </c>
       <c r="B107" s="13"/>
       <c r="C107" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="108" spans="1:3" outlineLevel="3">
       <c r="A108" s="8"/>
       <c r="B108" s="8"/>
       <c r="C108" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="109" spans="1:3" outlineLevel="3">
       <c r="A109" s="8"/>
       <c r="B109" s="8"/>
       <c r="C109" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="110" spans="1:3" outlineLevel="3">
       <c r="A110" s="8"/>
       <c r="B110" s="8"/>
       <c r="C110" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="111" spans="1:3" outlineLevel="3">
       <c r="A111" s="8"/>
       <c r="B111" s="8"/>
       <c r="C111" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="112" spans="1:3" outlineLevel="3">
       <c r="A112" s="8"/>
       <c r="B112" s="8"/>
       <c r="C112" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="113" spans="1:3" outlineLevel="3">
       <c r="A113" s="8"/>
       <c r="B113" s="8"/>
       <c r="C113" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="114" spans="1:3" outlineLevel="2">
@@ -3107,35 +3243,35 @@
       </c>
       <c r="B115" s="13"/>
       <c r="C115" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="116" spans="1:3" outlineLevel="3">
       <c r="A116" s="8"/>
       <c r="B116" s="8"/>
       <c r="C116" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="117" spans="1:3" outlineLevel="3">
       <c r="A117" s="8"/>
       <c r="B117" s="8"/>
       <c r="C117" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="118" spans="1:3" outlineLevel="3">
       <c r="A118" s="8"/>
       <c r="B118" s="8"/>
       <c r="C118" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="119" spans="1:3" outlineLevel="3">
       <c r="A119" s="6"/>
       <c r="B119" s="6"/>
       <c r="C119" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="120" spans="1:3" outlineLevel="2">
@@ -3149,35 +3285,35 @@
       </c>
       <c r="B121" s="13"/>
       <c r="C121" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="122" spans="1:3" outlineLevel="3">
       <c r="A122" s="8"/>
       <c r="B122" s="8"/>
       <c r="C122" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="123" spans="1:3" outlineLevel="3">
       <c r="A123" s="8"/>
       <c r="B123" s="8"/>
       <c r="C123" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="124" spans="1:3" outlineLevel="3">
       <c r="A124" s="8"/>
       <c r="B124" s="8"/>
       <c r="C124" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="125" spans="1:3" outlineLevel="3">
       <c r="A125" s="8"/>
       <c r="B125" s="8"/>
       <c r="C125" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="126" spans="1:3" outlineLevel="2">
@@ -3191,21 +3327,21 @@
       </c>
       <c r="B127" s="13"/>
       <c r="C127" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="128" spans="1:3" outlineLevel="3">
       <c r="A128" s="8"/>
       <c r="B128" s="8"/>
       <c r="C128" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="129" spans="1:3" outlineLevel="3">
       <c r="A129" s="8"/>
       <c r="B129" s="8"/>
       <c r="C129" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="130" spans="1:3" outlineLevel="1">
@@ -3219,7 +3355,7 @@
       </c>
       <c r="B131" s="7"/>
       <c r="C131" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="132" spans="1:3" outlineLevel="2">
@@ -3233,49 +3369,49 @@
       </c>
       <c r="B133" s="13"/>
       <c r="C133" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="134" spans="1:3" outlineLevel="3">
       <c r="A134" s="8"/>
       <c r="B134" s="8"/>
       <c r="C134" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="135" spans="1:3" outlineLevel="3">
       <c r="A135" s="8"/>
       <c r="B135" s="8"/>
       <c r="C135" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="136" spans="1:3" outlineLevel="3">
       <c r="A136" s="8"/>
       <c r="B136" s="8"/>
       <c r="C136" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="137" spans="1:3" outlineLevel="3">
       <c r="A137" s="8"/>
       <c r="B137" s="8"/>
       <c r="C137" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="138" spans="1:3" outlineLevel="3">
       <c r="A138" s="8"/>
       <c r="B138" s="8"/>
       <c r="C138" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="139" spans="1:3" outlineLevel="3">
       <c r="A139" s="8"/>
       <c r="B139" s="8"/>
       <c r="C139" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="140" spans="1:3" outlineLevel="2">
@@ -3289,28 +3425,28 @@
       </c>
       <c r="B141" s="13"/>
       <c r="C141" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="142" spans="1:3" outlineLevel="3">
       <c r="A142" s="8"/>
       <c r="B142" s="8"/>
       <c r="C142" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="143" spans="1:3" outlineLevel="3">
       <c r="A143" s="8"/>
       <c r="B143" s="8"/>
       <c r="C143" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="144" spans="1:3" outlineLevel="3">
       <c r="A144" s="8"/>
       <c r="B144" s="8"/>
       <c r="C144" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="145" spans="1:3" outlineLevel="2">
@@ -3324,42 +3460,42 @@
       </c>
       <c r="B146" s="13"/>
       <c r="C146" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="147" spans="1:3" outlineLevel="3">
       <c r="A147" s="8"/>
       <c r="B147" s="8"/>
       <c r="C147" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="148" spans="1:3" outlineLevel="3">
       <c r="A148" s="8"/>
       <c r="B148" s="8"/>
       <c r="C148" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="149" spans="1:3" outlineLevel="3">
       <c r="A149" s="8"/>
       <c r="B149" s="8"/>
       <c r="C149" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="150" spans="1:3" outlineLevel="3">
       <c r="A150" s="8"/>
       <c r="B150" s="8"/>
       <c r="C150" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="151" spans="1:3" outlineLevel="3">
       <c r="A151" s="8"/>
       <c r="B151" s="8"/>
       <c r="C151" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="152" spans="1:3" outlineLevel="2">
@@ -3373,35 +3509,35 @@
       </c>
       <c r="B153" s="13"/>
       <c r="C153" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="154" spans="1:3" outlineLevel="3">
       <c r="A154" s="8"/>
       <c r="B154" s="8"/>
       <c r="C154" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="155" spans="1:3" outlineLevel="3">
       <c r="A155" s="8"/>
       <c r="B155" s="8"/>
       <c r="C155" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="156" spans="1:3" outlineLevel="3">
       <c r="A156" s="8"/>
       <c r="B156" s="8"/>
       <c r="C156" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="157" spans="1:3" outlineLevel="3">
       <c r="A157" s="8"/>
       <c r="B157" s="8"/>
       <c r="C157" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="158" spans="1:3" outlineLevel="2">
@@ -3415,28 +3551,28 @@
       </c>
       <c r="B159" s="13"/>
       <c r="C159" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="160" spans="1:3" outlineLevel="3">
       <c r="A160" s="8"/>
       <c r="B160" s="8"/>
       <c r="C160" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="161" spans="1:3" outlineLevel="3">
       <c r="A161" s="8"/>
       <c r="B161" s="8"/>
       <c r="C161" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="162" spans="1:3" outlineLevel="3">
       <c r="A162" s="8"/>
       <c r="B162" s="8"/>
       <c r="C162" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="163" spans="1:3" outlineLevel="2">
@@ -3450,28 +3586,28 @@
       </c>
       <c r="B164" s="13"/>
       <c r="C164" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="165" spans="1:3" outlineLevel="3">
       <c r="A165" s="8"/>
       <c r="B165" s="8"/>
       <c r="C165" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="166" spans="1:3" outlineLevel="3">
       <c r="A166" s="8"/>
       <c r="B166" s="8"/>
       <c r="C166" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="167" spans="1:3" outlineLevel="3">
       <c r="A167" s="8"/>
       <c r="B167" s="8"/>
       <c r="C167" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -3513,49 +3649,49 @@
       </c>
       <c r="B173" s="13"/>
       <c r="C173" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="174" spans="1:3" outlineLevel="3">
       <c r="A174" s="8"/>
       <c r="B174" s="8"/>
       <c r="C174" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="175" spans="1:3" outlineLevel="3">
       <c r="A175" s="8"/>
       <c r="B175" s="8"/>
       <c r="C175" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="176" spans="1:3" outlineLevel="3">
       <c r="A176" s="8"/>
       <c r="B176" s="8"/>
       <c r="C176" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="177" spans="1:3" outlineLevel="3">
       <c r="A177" s="8"/>
       <c r="B177" s="8"/>
       <c r="C177" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="178" spans="1:3" outlineLevel="3">
       <c r="A178" s="8"/>
       <c r="B178" s="8"/>
       <c r="C178" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="179" spans="1:3" outlineLevel="3">
       <c r="A179" s="8"/>
       <c r="B179" s="8"/>
       <c r="C179" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="180" spans="1:3" outlineLevel="2">
@@ -3569,70 +3705,70 @@
       </c>
       <c r="B181" s="13"/>
       <c r="C181" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="182" spans="1:3" outlineLevel="3">
       <c r="A182" s="8"/>
       <c r="B182" s="8"/>
       <c r="C182" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="183" spans="1:3" outlineLevel="3">
       <c r="A183" s="8"/>
       <c r="B183" s="8"/>
       <c r="C183" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="184" spans="1:3" outlineLevel="3">
       <c r="A184" s="8"/>
       <c r="B184" s="8"/>
       <c r="C184" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="185" spans="1:3" outlineLevel="3">
       <c r="A185" s="8"/>
       <c r="B185" s="8"/>
       <c r="C185" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="186" spans="1:3" outlineLevel="3">
       <c r="A186" s="8"/>
       <c r="B186" s="8"/>
       <c r="C186" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="187" spans="1:3" outlineLevel="3">
       <c r="A187" s="8"/>
       <c r="B187" s="8"/>
       <c r="C187" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="188" spans="1:3" outlineLevel="3">
       <c r="A188" s="8"/>
       <c r="B188" s="8"/>
       <c r="C188" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="189" spans="1:3" outlineLevel="3">
       <c r="A189" s="8"/>
       <c r="B189" s="8"/>
       <c r="C189" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="190" spans="1:3" outlineLevel="3">
       <c r="A190" s="8"/>
       <c r="B190" s="8"/>
       <c r="C190" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="191" spans="1:3" outlineLevel="2">
@@ -3646,35 +3782,35 @@
       </c>
       <c r="B192" s="13"/>
       <c r="C192" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="193" spans="1:3" outlineLevel="3">
       <c r="A193" s="8"/>
       <c r="B193" s="8"/>
       <c r="C193" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="194" spans="1:3" outlineLevel="3">
       <c r="A194" s="8"/>
       <c r="B194" s="8"/>
       <c r="C194" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="195" spans="1:3" outlineLevel="3">
       <c r="A195" s="8"/>
       <c r="B195" s="8"/>
       <c r="C195" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="196" spans="1:3" outlineLevel="3">
       <c r="A196" s="8"/>
       <c r="B196" s="8"/>
       <c r="C196" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="197" spans="1:3" outlineLevel="2">
@@ -3688,49 +3824,49 @@
       </c>
       <c r="B198" s="13"/>
       <c r="C198" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="199" spans="1:3" outlineLevel="3">
       <c r="A199" s="8"/>
       <c r="B199" s="8"/>
       <c r="C199" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="200" spans="1:3" outlineLevel="3">
       <c r="A200" s="8"/>
       <c r="B200" s="8"/>
       <c r="C200" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="201" spans="1:3" outlineLevel="3">
       <c r="A201" s="8"/>
       <c r="B201" s="8"/>
       <c r="C201" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="202" spans="1:3" outlineLevel="3">
       <c r="A202" s="8"/>
       <c r="B202" s="8"/>
       <c r="C202" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="203" spans="1:3" outlineLevel="3">
       <c r="A203" s="8"/>
       <c r="B203" s="8"/>
       <c r="C203" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="204" spans="1:3" outlineLevel="3">
       <c r="A204" s="8"/>
       <c r="B204" s="8"/>
       <c r="C204" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="205" spans="1:3" outlineLevel="2">
@@ -3744,49 +3880,49 @@
       </c>
       <c r="B206" s="13"/>
       <c r="C206" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="207" spans="1:3" outlineLevel="3">
       <c r="A207" s="8"/>
       <c r="B207" s="8"/>
       <c r="C207" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="208" spans="1:3" outlineLevel="3">
       <c r="A208" s="8"/>
       <c r="B208" s="8"/>
       <c r="C208" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="209" spans="1:3" outlineLevel="3">
       <c r="A209" s="8"/>
       <c r="B209" s="8"/>
       <c r="C209" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="210" spans="1:3" outlineLevel="3">
       <c r="A210" s="8"/>
       <c r="B210" s="8"/>
       <c r="C210" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="211" spans="1:3" outlineLevel="3">
       <c r="A211" s="8"/>
       <c r="B211" s="8"/>
       <c r="C211" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="212" spans="1:3" outlineLevel="3">
       <c r="A212" s="8"/>
       <c r="B212" s="8"/>
       <c r="C212" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="213" spans="1:3" outlineLevel="1">
@@ -3814,63 +3950,63 @@
       </c>
       <c r="B216" s="13"/>
       <c r="C216" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="217" spans="1:3" outlineLevel="3">
       <c r="A217" s="6"/>
       <c r="B217" s="6"/>
       <c r="C217" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="218" spans="1:3" outlineLevel="3">
       <c r="A218" s="6"/>
       <c r="B218" s="6"/>
       <c r="C218" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="219" spans="1:3" outlineLevel="3">
       <c r="A219" s="6"/>
       <c r="B219" s="6"/>
       <c r="C219" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="220" spans="1:3" outlineLevel="3">
       <c r="A220" s="6"/>
       <c r="B220" s="6"/>
       <c r="C220" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="221" spans="1:3" outlineLevel="3">
       <c r="A221" s="6"/>
       <c r="B221" s="6"/>
       <c r="C221" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="222" spans="1:3" outlineLevel="3">
       <c r="A222" s="6"/>
       <c r="B222" s="6"/>
       <c r="C222" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="223" spans="1:3" outlineLevel="3">
       <c r="A223" s="6"/>
       <c r="B223" s="6"/>
       <c r="C223" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="224" spans="1:3" outlineLevel="3">
       <c r="A224" s="6"/>
       <c r="B224" s="6"/>
       <c r="C224" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="225" spans="1:3" outlineLevel="2">
@@ -3884,42 +4020,42 @@
       </c>
       <c r="B226" s="13"/>
       <c r="C226" s="12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="227" spans="1:3" outlineLevel="3">
       <c r="A227" s="6"/>
       <c r="B227" s="6"/>
       <c r="C227" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="228" spans="1:3" outlineLevel="3">
       <c r="A228" s="6"/>
       <c r="B228" s="6"/>
       <c r="C228" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="229" spans="1:3" outlineLevel="3">
       <c r="A229" s="6"/>
       <c r="B229" s="6"/>
       <c r="C229" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="230" spans="1:3" outlineLevel="3">
       <c r="A230" s="6"/>
       <c r="B230" s="6"/>
       <c r="C230" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="231" spans="1:3" outlineLevel="3">
       <c r="A231" s="6"/>
       <c r="B231" s="6"/>
       <c r="C231" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="232" spans="1:3" outlineLevel="2">
@@ -3933,42 +4069,42 @@
       </c>
       <c r="B233" s="13"/>
       <c r="C233" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="234" spans="1:3" outlineLevel="3">
       <c r="A234" s="6"/>
       <c r="B234" s="6"/>
       <c r="C234" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="235" spans="1:3" outlineLevel="3">
       <c r="A235" s="6"/>
       <c r="B235" s="6"/>
       <c r="C235" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="236" spans="1:3" outlineLevel="3">
       <c r="A236" s="6"/>
       <c r="B236" s="6"/>
       <c r="C236" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="237" spans="1:3" outlineLevel="3">
       <c r="A237" s="6"/>
       <c r="B237" s="6"/>
       <c r="C237" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="238" spans="1:3" outlineLevel="3">
       <c r="A238" s="6"/>
       <c r="B238" s="6"/>
       <c r="C238" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="239" spans="1:3" outlineLevel="2">
@@ -3982,28 +4118,28 @@
       </c>
       <c r="B240" s="13"/>
       <c r="C240" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="241" spans="1:3" outlineLevel="3">
       <c r="A241" s="6"/>
       <c r="B241" s="6"/>
       <c r="C241" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="242" spans="1:3" outlineLevel="3">
       <c r="A242" s="6"/>
       <c r="B242" s="6"/>
       <c r="C242" s="10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="243" spans="1:3" outlineLevel="3">
       <c r="A243" s="6"/>
       <c r="B243" s="6"/>
       <c r="C243" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="244" spans="1:3" outlineLevel="2">
@@ -4017,35 +4153,35 @@
       </c>
       <c r="B245" s="13"/>
       <c r="C245" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="246" spans="1:3" outlineLevel="3">
       <c r="A246" s="6"/>
       <c r="B246" s="6"/>
       <c r="C246" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="247" spans="1:3" outlineLevel="3">
       <c r="A247" s="6"/>
       <c r="B247" s="6"/>
       <c r="C247" s="10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="248" spans="1:3" outlineLevel="3">
       <c r="A248" s="6"/>
       <c r="B248" s="6"/>
       <c r="C248" s="10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="249" spans="1:3" outlineLevel="3">
       <c r="A249" s="6"/>
       <c r="B249" s="6"/>
       <c r="C249" s="10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="250" spans="1:3" outlineLevel="2">
@@ -4059,28 +4195,28 @@
       </c>
       <c r="B251" s="13"/>
       <c r="C251" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="252" spans="1:3" outlineLevel="3">
       <c r="A252" s="6"/>
       <c r="B252" s="6"/>
       <c r="C252" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="253" spans="1:3" outlineLevel="3">
       <c r="A253" s="6"/>
       <c r="B253" s="6"/>
       <c r="C253" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="254" spans="1:3" outlineLevel="3">
       <c r="A254" s="6"/>
       <c r="B254" s="6"/>
       <c r="C254" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="255" spans="1:3" outlineLevel="2">
@@ -4094,42 +4230,42 @@
       </c>
       <c r="B256" s="13"/>
       <c r="C256" s="12" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="257" spans="1:3" outlineLevel="3">
       <c r="A257" s="6"/>
       <c r="B257" s="6"/>
       <c r="C257" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="258" spans="1:3" outlineLevel="3">
       <c r="A258" s="6"/>
       <c r="B258" s="6"/>
       <c r="C258" s="10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="259" spans="1:3" outlineLevel="3">
       <c r="A259" s="6"/>
       <c r="B259" s="6"/>
       <c r="C259" s="10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="260" spans="1:3" outlineLevel="3">
       <c r="A260" s="6"/>
       <c r="B260" s="6"/>
       <c r="C260" s="10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="261" spans="1:3" outlineLevel="3">
       <c r="A261" s="6"/>
       <c r="B261" s="6"/>
       <c r="C261" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="262" spans="1:3" outlineLevel="2">
@@ -4143,35 +4279,35 @@
       </c>
       <c r="B263" s="13"/>
       <c r="C263" s="12" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="264" spans="1:3" outlineLevel="3">
       <c r="A264" s="6"/>
       <c r="B264" s="6"/>
       <c r="C264" s="10" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="265" spans="1:3" outlineLevel="3">
       <c r="A265" s="6"/>
       <c r="B265" s="6"/>
       <c r="C265" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="266" spans="1:3" outlineLevel="3">
       <c r="A266" s="6"/>
       <c r="B266" s="6"/>
       <c r="C266" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="267" spans="1:3" outlineLevel="3">
       <c r="A267" s="6"/>
       <c r="B267" s="6"/>
       <c r="C267" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="268" spans="1:3" outlineLevel="2">
@@ -4185,35 +4321,35 @@
       </c>
       <c r="B269" s="13"/>
       <c r="C269" s="12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="270" spans="1:3" outlineLevel="3">
       <c r="A270" s="6"/>
       <c r="B270" s="6"/>
       <c r="C270" s="10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="271" spans="1:3" outlineLevel="3">
       <c r="A271" s="6"/>
       <c r="B271" s="6"/>
       <c r="C271" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="272" spans="1:3" outlineLevel="3">
       <c r="A272" s="6"/>
       <c r="B272" s="6"/>
       <c r="C272" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="273" spans="1:3" outlineLevel="3">
       <c r="A273" s="6"/>
       <c r="B273" s="6"/>
       <c r="C273" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="274" spans="1:3" outlineLevel="2">
@@ -4227,35 +4363,35 @@
       </c>
       <c r="B275" s="13"/>
       <c r="C275" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="276" spans="1:3" outlineLevel="3">
       <c r="A276" s="6"/>
       <c r="B276" s="6"/>
       <c r="C276" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="277" spans="1:3" outlineLevel="3">
       <c r="A277" s="6"/>
       <c r="B277" s="6"/>
       <c r="C277" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="278" spans="1:3" outlineLevel="3">
       <c r="A278" s="6"/>
       <c r="B278" s="6"/>
       <c r="C278" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="279" spans="1:3" outlineLevel="3">
       <c r="A279" s="6"/>
       <c r="B279" s="6"/>
       <c r="C279" s="10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="280" spans="1:3" outlineLevel="1">
@@ -4283,7 +4419,7 @@
       </c>
       <c r="B283" s="13"/>
       <c r="C283" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="284" spans="1:3" outlineLevel="2">
@@ -4297,7 +4433,7 @@
       </c>
       <c r="B285" s="13"/>
       <c r="C285" s="12" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="286" spans="1:3" outlineLevel="2">
@@ -4311,7 +4447,7 @@
       </c>
       <c r="B287" s="13"/>
       <c r="C287" s="12" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="288" spans="1:3">
@@ -4353,21 +4489,21 @@
       </c>
       <c r="B293" s="13"/>
       <c r="C293" s="12" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="294" spans="1:3" outlineLevel="3">
       <c r="A294" s="8"/>
       <c r="B294" s="8"/>
       <c r="C294" s="9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="295" spans="1:3" outlineLevel="3">
       <c r="A295" s="8"/>
       <c r="B295" s="8"/>
       <c r="C295" s="9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="296" spans="1:3" outlineLevel="2">
@@ -4381,14 +4517,14 @@
       </c>
       <c r="B297" s="13"/>
       <c r="C297" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="298" spans="1:3" outlineLevel="3">
       <c r="A298" s="8"/>
       <c r="B298" s="8"/>
       <c r="C298" s="9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="299" spans="1:3" outlineLevel="2">
@@ -4402,35 +4538,35 @@
       </c>
       <c r="B300" s="13"/>
       <c r="C300" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="301" spans="1:3" outlineLevel="3">
       <c r="A301" s="8"/>
       <c r="B301" s="8"/>
       <c r="C301" s="9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="302" spans="1:3" outlineLevel="3">
       <c r="A302" s="8"/>
       <c r="B302" s="8"/>
       <c r="C302" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="303" spans="1:3" outlineLevel="3">
       <c r="A303" s="8"/>
       <c r="B303" s="8"/>
       <c r="C303" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="304" spans="1:3" outlineLevel="3">
       <c r="A304" s="8"/>
       <c r="B304" s="8"/>
       <c r="C304" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="305" spans="1:3" outlineLevel="2">
@@ -4444,21 +4580,21 @@
       </c>
       <c r="B306" s="13"/>
       <c r="C306" s="12" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="307" spans="1:3" outlineLevel="3">
       <c r="A307" s="8"/>
       <c r="B307" s="8"/>
       <c r="C307" s="9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="308" spans="1:3" outlineLevel="3">
       <c r="A308" s="8"/>
       <c r="B308" s="8"/>
       <c r="C308" s="9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="309" spans="1:3" outlineLevel="2">
@@ -4472,28 +4608,28 @@
       </c>
       <c r="B310" s="13"/>
       <c r="C310" s="12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="311" spans="1:3" outlineLevel="3">
       <c r="A311" s="8"/>
       <c r="B311" s="8"/>
       <c r="C311" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="312" spans="1:3" outlineLevel="3">
       <c r="A312" s="8"/>
       <c r="B312" s="8"/>
       <c r="C312" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="313" spans="1:3" outlineLevel="3">
       <c r="A313" s="8"/>
       <c r="B313" s="8"/>
       <c r="C313" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="314" spans="1:3" outlineLevel="2">
@@ -4507,28 +4643,28 @@
       </c>
       <c r="B315" s="13"/>
       <c r="C315" s="12" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="316" spans="1:3" outlineLevel="3">
       <c r="A316" s="8"/>
       <c r="B316" s="8"/>
       <c r="C316" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="317" spans="1:3" outlineLevel="3">
       <c r="A317" s="8"/>
       <c r="B317" s="8"/>
       <c r="C317" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="318" spans="1:3" outlineLevel="3">
       <c r="A318" s="8"/>
       <c r="B318" s="8"/>
       <c r="C318" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="319" spans="1:3" outlineLevel="2">
@@ -4542,35 +4678,35 @@
       </c>
       <c r="B320" s="13"/>
       <c r="C320" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="321" spans="1:3" outlineLevel="3">
       <c r="A321" s="8"/>
       <c r="B321" s="8"/>
       <c r="C321" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="322" spans="1:3" outlineLevel="3">
       <c r="A322" s="8"/>
       <c r="B322" s="8"/>
       <c r="C322" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="323" spans="1:3" outlineLevel="3">
       <c r="A323" s="8"/>
       <c r="B323" s="8"/>
       <c r="C323" s="9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="324" spans="1:3" outlineLevel="3">
       <c r="A324" s="8"/>
       <c r="B324" s="8"/>
       <c r="C324" s="9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="325" spans="1:3" outlineLevel="1">
@@ -4598,70 +4734,70 @@
       </c>
       <c r="B328" s="13"/>
       <c r="C328" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="329" spans="1:3" outlineLevel="3">
       <c r="A329" s="8"/>
       <c r="B329" s="8"/>
       <c r="C329" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="330" spans="1:3" outlineLevel="3">
       <c r="A330" s="8"/>
       <c r="B330" s="8"/>
       <c r="C330" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="331" spans="1:3" outlineLevel="3">
       <c r="A331" s="8"/>
       <c r="B331" s="8"/>
       <c r="C331" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="332" spans="1:3" outlineLevel="3">
       <c r="A332" s="8"/>
       <c r="B332" s="8"/>
       <c r="C332" s="9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="333" spans="1:3" outlineLevel="3">
       <c r="A333" s="8"/>
       <c r="B333" s="8"/>
       <c r="C333" s="9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="334" spans="1:3" outlineLevel="3">
       <c r="A334" s="8"/>
       <c r="B334" s="8"/>
       <c r="C334" s="9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="335" spans="1:3" outlineLevel="3">
       <c r="A335" s="8"/>
       <c r="B335" s="8"/>
       <c r="C335" s="9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="336" spans="1:3" outlineLevel="3">
       <c r="A336" s="8"/>
       <c r="B336" s="8"/>
       <c r="C336" s="9" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="337" spans="1:3" outlineLevel="3">
       <c r="A337" s="8"/>
       <c r="B337" s="8"/>
       <c r="C337" s="9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="338" spans="1:3" outlineLevel="2">
@@ -4675,49 +4811,49 @@
       </c>
       <c r="B339" s="13"/>
       <c r="C339" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="340" spans="1:3" outlineLevel="3">
       <c r="A340" s="8"/>
       <c r="B340" s="8"/>
       <c r="C340" s="9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="341" spans="1:3" outlineLevel="3">
       <c r="A341" s="8"/>
       <c r="B341" s="8"/>
       <c r="C341" s="9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="342" spans="1:3" outlineLevel="3">
       <c r="A342" s="8"/>
       <c r="B342" s="8"/>
       <c r="C342" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="343" spans="1:3" outlineLevel="3">
       <c r="A343" s="8"/>
       <c r="B343" s="8"/>
       <c r="C343" s="9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="344" spans="1:3" outlineLevel="3">
       <c r="A344" s="8"/>
       <c r="B344" s="8"/>
       <c r="C344" s="9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="345" spans="1:3" outlineLevel="3">
       <c r="A345" s="8"/>
       <c r="B345" s="8"/>
       <c r="C345" s="9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="346" spans="1:3" outlineLevel="2">
@@ -4731,28 +4867,28 @@
       </c>
       <c r="B347" s="13"/>
       <c r="C347" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="348" spans="1:3" outlineLevel="3">
       <c r="A348" s="8"/>
       <c r="B348" s="8"/>
       <c r="C348" s="9" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="349" spans="1:3" outlineLevel="3">
       <c r="A349" s="8"/>
       <c r="B349" s="8"/>
       <c r="C349" s="9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="350" spans="1:3" outlineLevel="3">
       <c r="A350" s="8"/>
       <c r="B350" s="8"/>
       <c r="C350" s="9" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="351" spans="1:3" outlineLevel="2">
@@ -4766,42 +4902,42 @@
       </c>
       <c r="B352" s="13"/>
       <c r="C352" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="353" spans="1:3" outlineLevel="3">
       <c r="A353" s="8"/>
       <c r="B353" s="8"/>
       <c r="C353" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="354" spans="1:3" outlineLevel="3">
       <c r="A354" s="8"/>
       <c r="B354" s="8"/>
       <c r="C354" s="9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="355" spans="1:3" outlineLevel="3">
       <c r="A355" s="8"/>
       <c r="B355" s="8"/>
       <c r="C355" s="9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="356" spans="1:3" outlineLevel="3">
       <c r="A356" s="8"/>
       <c r="B356" s="8"/>
       <c r="C356" s="9" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="357" spans="1:3" outlineLevel="3">
       <c r="A357" s="8"/>
       <c r="B357" s="8"/>
       <c r="C357" s="9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="358" spans="1:3" outlineLevel="2">
@@ -4815,28 +4951,28 @@
       </c>
       <c r="B359" s="13"/>
       <c r="C359" s="12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="360" spans="1:3" outlineLevel="3">
       <c r="A360" s="8"/>
       <c r="B360" s="8"/>
       <c r="C360" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="361" spans="1:3" outlineLevel="3">
       <c r="A361" s="8"/>
       <c r="B361" s="8"/>
       <c r="C361" s="9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="362" spans="1:3" outlineLevel="3">
       <c r="A362" s="8"/>
       <c r="B362" s="8"/>
       <c r="C362" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="363" spans="1:3" outlineLevel="2">
@@ -4850,35 +4986,35 @@
       </c>
       <c r="B364" s="13"/>
       <c r="C364" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="365" spans="1:3" outlineLevel="3">
       <c r="A365" s="8"/>
       <c r="B365" s="8"/>
       <c r="C365" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="366" spans="1:3" outlineLevel="3">
       <c r="A366" s="8"/>
       <c r="B366" s="8"/>
       <c r="C366" s="9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="367" spans="1:3" outlineLevel="3">
       <c r="A367" s="8"/>
       <c r="B367" s="8"/>
       <c r="C367" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="368" spans="1:3" outlineLevel="3">
       <c r="A368" s="8"/>
       <c r="B368" s="8"/>
       <c r="C368" s="9" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="369" spans="1:3" outlineLevel="2">
@@ -4892,35 +5028,35 @@
       </c>
       <c r="B370" s="13"/>
       <c r="C370" s="12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="371" spans="1:3" outlineLevel="3">
       <c r="A371" s="8"/>
       <c r="B371" s="8"/>
       <c r="C371" s="9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="372" spans="1:3" outlineLevel="3">
       <c r="A372" s="8"/>
       <c r="B372" s="8"/>
       <c r="C372" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="373" spans="1:3" outlineLevel="3">
       <c r="A373" s="8"/>
       <c r="B373" s="8"/>
       <c r="C373" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="374" spans="1:3" outlineLevel="3">
       <c r="A374" s="8"/>
       <c r="B374" s="8"/>
       <c r="C374" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="375" spans="1:3" outlineLevel="1">
@@ -4948,105 +5084,105 @@
       </c>
       <c r="B378" s="13"/>
       <c r="C378" s="12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="379" spans="1:3" outlineLevel="3">
       <c r="A379" s="8"/>
       <c r="B379" s="8"/>
       <c r="C379" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="380" spans="1:3" outlineLevel="3">
       <c r="A380" s="8"/>
       <c r="B380" s="8"/>
       <c r="C380" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="381" spans="1:3" outlineLevel="3">
       <c r="A381" s="8"/>
       <c r="B381" s="8"/>
       <c r="C381" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="382" spans="1:3" outlineLevel="3">
       <c r="A382" s="8"/>
       <c r="B382" s="8"/>
       <c r="C382" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="383" spans="1:3" outlineLevel="3">
       <c r="A383" s="8"/>
       <c r="B383" s="8"/>
       <c r="C383" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="384" spans="1:3" outlineLevel="3">
       <c r="A384" s="8"/>
       <c r="B384" s="8"/>
       <c r="C384" s="9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="385" spans="1:3" outlineLevel="3">
       <c r="A385" s="8"/>
       <c r="B385" s="8"/>
       <c r="C385" s="9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="386" spans="1:3" outlineLevel="3">
       <c r="A386" s="8"/>
       <c r="B386" s="8"/>
       <c r="C386" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="387" spans="1:3" outlineLevel="3">
       <c r="A387" s="8"/>
       <c r="B387" s="8"/>
       <c r="C387" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="388" spans="1:3" outlineLevel="3">
       <c r="A388" s="8"/>
       <c r="B388" s="8"/>
       <c r="C388" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="389" spans="1:3" outlineLevel="3">
       <c r="A389" s="8"/>
       <c r="B389" s="8"/>
       <c r="C389" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="390" spans="1:3" outlineLevel="3">
       <c r="A390" s="8"/>
       <c r="B390" s="8"/>
       <c r="C390" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="391" spans="1:3" outlineLevel="3">
       <c r="A391" s="8"/>
       <c r="B391" s="8"/>
       <c r="C391" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="392" spans="1:3" outlineLevel="3">
       <c r="A392" s="8"/>
       <c r="B392" s="8"/>
       <c r="C392" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="393" spans="1:3" outlineLevel="2">
@@ -5060,49 +5196,49 @@
       </c>
       <c r="B394" s="13"/>
       <c r="C394" s="12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="395" spans="1:3" outlineLevel="3">
       <c r="A395" s="8"/>
       <c r="B395" s="8"/>
       <c r="C395" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="396" spans="1:3" outlineLevel="3">
       <c r="A396" s="8"/>
       <c r="B396" s="8"/>
       <c r="C396" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="397" spans="1:3" outlineLevel="3">
       <c r="A397" s="8"/>
       <c r="B397" s="8"/>
       <c r="C397" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="398" spans="1:3" outlineLevel="3">
       <c r="A398" s="8"/>
       <c r="B398" s="8"/>
       <c r="C398" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="399" spans="1:3" outlineLevel="3">
       <c r="A399" s="8"/>
       <c r="B399" s="8"/>
       <c r="C399" s="9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="400" spans="1:3" outlineLevel="3">
       <c r="A400" s="8"/>
       <c r="B400" s="8"/>
       <c r="C400" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="401" spans="1:3" outlineLevel="2">
@@ -5116,42 +5252,42 @@
       </c>
       <c r="B402" s="13"/>
       <c r="C402" s="12" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="403" spans="1:3" outlineLevel="3">
       <c r="A403" s="8"/>
       <c r="B403" s="8"/>
       <c r="C403" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="404" spans="1:3" outlineLevel="3">
       <c r="A404" s="8"/>
       <c r="B404" s="8"/>
       <c r="C404" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="405" spans="1:3" outlineLevel="3">
       <c r="A405" s="8"/>
       <c r="B405" s="8"/>
       <c r="C405" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="406" spans="1:3" outlineLevel="3">
       <c r="A406" s="8"/>
       <c r="B406" s="8"/>
       <c r="C406" s="9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="407" spans="1:3" outlineLevel="3">
       <c r="A407" s="8"/>
       <c r="B407" s="8"/>
       <c r="C407" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="408" spans="1:3" outlineLevel="2">
@@ -5165,63 +5301,63 @@
       </c>
       <c r="B409" s="13"/>
       <c r="C409" s="12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="410" spans="1:3" outlineLevel="3">
       <c r="A410" s="8"/>
       <c r="B410" s="8"/>
       <c r="C410" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="411" spans="1:3" outlineLevel="3">
       <c r="A411" s="8"/>
       <c r="B411" s="8"/>
       <c r="C411" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="412" spans="1:3" outlineLevel="3">
       <c r="A412" s="8"/>
       <c r="B412" s="8"/>
       <c r="C412" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="413" spans="1:3" outlineLevel="3">
       <c r="A413" s="8"/>
       <c r="B413" s="8"/>
       <c r="C413" s="9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="414" spans="1:3" outlineLevel="3">
       <c r="A414" s="8"/>
       <c r="B414" s="8"/>
       <c r="C414" s="9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="415" spans="1:3" outlineLevel="3">
       <c r="A415" s="8"/>
       <c r="B415" s="8"/>
       <c r="C415" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="416" spans="1:3" outlineLevel="3">
       <c r="A416" s="8"/>
       <c r="B416" s="8"/>
       <c r="C416" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="417" spans="1:3" outlineLevel="3">
       <c r="A417" s="8"/>
       <c r="B417" s="8"/>
       <c r="C417" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="418" spans="1:3" outlineLevel="1">
@@ -5249,70 +5385,70 @@
       </c>
       <c r="B421" s="13"/>
       <c r="C421" s="12" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="422" spans="1:3" outlineLevel="3">
       <c r="A422" s="8"/>
       <c r="B422" s="8"/>
       <c r="C422" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="423" spans="1:3" outlineLevel="3">
       <c r="A423" s="8"/>
       <c r="B423" s="8"/>
       <c r="C423" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="424" spans="1:3" outlineLevel="3">
       <c r="A424" s="8"/>
       <c r="B424" s="8"/>
       <c r="C424" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="425" spans="1:3" outlineLevel="3">
       <c r="A425" s="8"/>
       <c r="B425" s="8"/>
       <c r="C425" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="426" spans="1:3" outlineLevel="3">
       <c r="A426" s="8"/>
       <c r="B426" s="8"/>
       <c r="C426" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="427" spans="1:3" outlineLevel="3">
       <c r="A427" s="8"/>
       <c r="B427" s="8"/>
       <c r="C427" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="428" spans="1:3" outlineLevel="3">
       <c r="A428" s="8"/>
       <c r="B428" s="8"/>
       <c r="C428" s="9" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="429" spans="1:3" outlineLevel="3">
       <c r="A429" s="8"/>
       <c r="B429" s="8"/>
       <c r="C429" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="430" spans="1:3" outlineLevel="3">
       <c r="A430" s="8"/>
       <c r="B430" s="8"/>
       <c r="C430" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="431" spans="1:3" outlineLevel="2">
@@ -5326,28 +5462,28 @@
       </c>
       <c r="B432" s="13"/>
       <c r="C432" s="12" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="433" spans="1:3" outlineLevel="3">
       <c r="A433" s="8"/>
       <c r="B433" s="8"/>
       <c r="C433" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="434" spans="1:3" outlineLevel="3">
       <c r="A434" s="8"/>
       <c r="B434" s="8"/>
       <c r="C434" s="9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="435" spans="1:3" outlineLevel="3">
       <c r="A435" s="8"/>
       <c r="B435" s="8"/>
       <c r="C435" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="436" spans="1:3" outlineLevel="2">
@@ -5361,35 +5497,35 @@
       </c>
       <c r="B437" s="13"/>
       <c r="C437" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="438" spans="1:3" outlineLevel="3">
       <c r="A438" s="8"/>
       <c r="B438" s="8"/>
       <c r="C438" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="439" spans="1:3" outlineLevel="3">
       <c r="A439" s="8"/>
       <c r="B439" s="8"/>
       <c r="C439" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="440" spans="1:3" outlineLevel="3">
       <c r="A440" s="8"/>
       <c r="B440" s="8"/>
       <c r="C440" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="441" spans="1:3" outlineLevel="3">
       <c r="A441" s="8"/>
       <c r="B441" s="8"/>
       <c r="C441" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="442" spans="1:3" outlineLevel="2">
@@ -5403,42 +5539,42 @@
       </c>
       <c r="B443" s="13"/>
       <c r="C443" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="444" spans="1:3" outlineLevel="3">
       <c r="A444" s="8"/>
       <c r="B444" s="8"/>
       <c r="C444" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="445" spans="1:3" outlineLevel="3">
       <c r="A445" s="8"/>
       <c r="B445" s="8"/>
       <c r="C445" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="446" spans="1:3" outlineLevel="3">
       <c r="A446" s="8"/>
       <c r="B446" s="8"/>
       <c r="C446" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="447" spans="1:3" outlineLevel="3">
       <c r="A447" s="8"/>
       <c r="B447" s="8"/>
       <c r="C447" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="448" spans="1:3" outlineLevel="3">
       <c r="A448" s="8"/>
       <c r="B448" s="8"/>
       <c r="C448" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="449" spans="1:3" outlineLevel="2">
@@ -5452,42 +5588,42 @@
       </c>
       <c r="B450" s="13"/>
       <c r="C450" s="12" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="451" spans="1:3" outlineLevel="3">
       <c r="A451" s="8"/>
       <c r="B451" s="8"/>
       <c r="C451" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="452" spans="1:3" outlineLevel="3">
       <c r="A452" s="8"/>
       <c r="B452" s="8"/>
       <c r="C452" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="453" spans="1:3" outlineLevel="3">
       <c r="A453" s="8"/>
       <c r="B453" s="8"/>
       <c r="C453" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="454" spans="1:3" outlineLevel="3">
       <c r="A454" s="8"/>
       <c r="B454" s="8"/>
       <c r="C454" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="455" spans="1:3" outlineLevel="3">
       <c r="A455" s="8"/>
       <c r="B455" s="8"/>
       <c r="C455" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="456" spans="1:3" outlineLevel="2">
@@ -5501,84 +5637,84 @@
       </c>
       <c r="B457" s="13"/>
       <c r="C457" s="12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="458" spans="1:3" outlineLevel="3">
       <c r="A458" s="8"/>
       <c r="B458" s="8"/>
       <c r="C458" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="459" spans="1:3" outlineLevel="3">
       <c r="A459" s="8"/>
       <c r="B459" s="8"/>
       <c r="C459" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="460" spans="1:3" outlineLevel="3">
       <c r="A460" s="8"/>
       <c r="B460" s="8"/>
       <c r="C460" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="461" spans="1:3" outlineLevel="3">
       <c r="A461" s="8"/>
       <c r="B461" s="8"/>
       <c r="C461" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="462" spans="1:3" outlineLevel="3">
       <c r="A462" s="8"/>
       <c r="B462" s="8"/>
       <c r="C462" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="463" spans="1:3" outlineLevel="3">
       <c r="A463" s="8"/>
       <c r="B463" s="8"/>
       <c r="C463" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="464" spans="1:3" outlineLevel="3">
       <c r="A464" s="8"/>
       <c r="B464" s="8"/>
       <c r="C464" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="465" spans="1:3" outlineLevel="3">
       <c r="A465" s="8"/>
       <c r="B465" s="8"/>
       <c r="C465" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="466" spans="1:3" outlineLevel="3">
       <c r="A466" s="8"/>
       <c r="B466" s="8"/>
       <c r="C466" s="9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="467" spans="1:3" outlineLevel="3">
       <c r="A467" s="8"/>
       <c r="B467" s="8"/>
       <c r="C467" s="9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="468" spans="1:3" outlineLevel="3">
       <c r="A468" s="8"/>
       <c r="B468" s="8"/>
       <c r="C468" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="469" spans="1:3" outlineLevel="1">
@@ -5606,49 +5742,49 @@
       </c>
       <c r="B472" s="13"/>
       <c r="C472" s="12" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="473" spans="1:3" outlineLevel="3">
       <c r="A473" s="8"/>
       <c r="B473" s="8"/>
       <c r="C473" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="474" spans="1:3" outlineLevel="3">
       <c r="A474" s="8"/>
       <c r="B474" s="8"/>
       <c r="C474" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="475" spans="1:3" outlineLevel="3">
       <c r="A475" s="8"/>
       <c r="B475" s="8"/>
-      <c r="C475" s="16" t="s">
-        <v>497</v>
+      <c r="C475" s="9" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="476" spans="1:3" outlineLevel="3">
       <c r="A476" s="8"/>
       <c r="B476" s="8"/>
       <c r="C476" s="9" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="477" spans="1:3" outlineLevel="3">
       <c r="A477" s="8"/>
       <c r="B477" s="8"/>
       <c r="C477" s="9" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="478" spans="1:3" outlineLevel="3">
       <c r="A478" s="8"/>
       <c r="B478" s="8"/>
       <c r="C478" s="9" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="479" spans="1:3" outlineLevel="2">
@@ -5662,28 +5798,28 @@
       </c>
       <c r="B480" s="13"/>
       <c r="C480" s="12" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="481" spans="1:3" outlineLevel="3">
       <c r="A481" s="8"/>
       <c r="B481" s="8"/>
       <c r="C481" s="9" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="482" spans="1:3" outlineLevel="3">
       <c r="A482" s="8"/>
       <c r="B482" s="8"/>
       <c r="C482" s="9" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="483" spans="1:3" outlineLevel="3">
       <c r="A483" s="8"/>
       <c r="B483" s="8"/>
       <c r="C483" s="9" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="484" spans="1:3" outlineLevel="2">
@@ -5697,42 +5833,42 @@
       </c>
       <c r="B485" s="13"/>
       <c r="C485" s="12" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="486" spans="1:3" outlineLevel="3">
       <c r="A486" s="8"/>
       <c r="B486" s="8"/>
       <c r="C486" s="9" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="487" spans="1:3" outlineLevel="3">
       <c r="A487" s="8"/>
       <c r="B487" s="8"/>
       <c r="C487" s="9" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="488" spans="1:3" outlineLevel="3">
       <c r="A488" s="8"/>
       <c r="B488" s="8"/>
       <c r="C488" s="9" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="489" spans="1:3" outlineLevel="3">
       <c r="A489" s="8"/>
       <c r="B489" s="8"/>
       <c r="C489" s="9" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="490" spans="1:3" outlineLevel="3">
       <c r="A490" s="8"/>
       <c r="B490" s="8"/>
       <c r="C490" s="9" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="491" spans="1:3" outlineLevel="2">
@@ -5746,28 +5882,28 @@
       </c>
       <c r="B492" s="13"/>
       <c r="C492" s="12" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="493" spans="1:3" outlineLevel="3">
       <c r="A493" s="8"/>
       <c r="B493" s="8"/>
       <c r="C493" s="9" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="494" spans="1:3" outlineLevel="3">
       <c r="A494" s="8"/>
       <c r="B494" s="8"/>
       <c r="C494" s="9" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="495" spans="1:3" outlineLevel="3">
       <c r="A495" s="8"/>
       <c r="B495" s="8"/>
       <c r="C495" s="9" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="496" spans="1:3" outlineLevel="2">
@@ -5781,35 +5917,35 @@
       </c>
       <c r="B497" s="13"/>
       <c r="C497" s="12" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="498" spans="1:3" outlineLevel="3">
       <c r="A498" s="8"/>
       <c r="B498" s="8"/>
       <c r="C498" s="9" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="499" spans="1:3" outlineLevel="3">
       <c r="A499" s="8"/>
       <c r="B499" s="8"/>
       <c r="C499" s="9" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="500" spans="1:3" outlineLevel="3">
       <c r="A500" s="8"/>
       <c r="B500" s="8"/>
       <c r="C500" s="9" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="501" spans="1:3" outlineLevel="3">
       <c r="A501" s="8"/>
       <c r="B501" s="8"/>
       <c r="C501" s="9" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="502" spans="1:3" outlineLevel="2">
@@ -5823,63 +5959,63 @@
       </c>
       <c r="B503" s="13"/>
       <c r="C503" s="12" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="504" spans="1:3" outlineLevel="3">
       <c r="A504" s="8"/>
       <c r="B504" s="8"/>
-      <c r="C504" s="16" t="s">
-        <v>114</v>
+      <c r="C504" s="9" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="505" spans="1:3" outlineLevel="3">
       <c r="A505" s="8"/>
       <c r="B505" s="8"/>
       <c r="C505" s="9" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="506" spans="1:3" outlineLevel="3">
       <c r="A506" s="8"/>
       <c r="B506" s="8"/>
       <c r="C506" s="9" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="507" spans="1:3" outlineLevel="3">
       <c r="A507" s="8"/>
       <c r="B507" s="8"/>
       <c r="C507" s="9" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="508" spans="1:3" outlineLevel="3">
       <c r="A508" s="8"/>
       <c r="B508" s="8"/>
       <c r="C508" s="9" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="509" spans="1:3" outlineLevel="3">
       <c r="A509" s="8"/>
       <c r="B509" s="8"/>
       <c r="C509" s="9" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="510" spans="1:3" outlineLevel="3">
       <c r="A510" s="8"/>
       <c r="B510" s="8"/>
       <c r="C510" s="9" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="511" spans="1:3" outlineLevel="3">
       <c r="A511" s="8"/>
       <c r="B511" s="8"/>
       <c r="C511" s="9" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="512" spans="1:3" outlineLevel="1">
@@ -5889,11 +6025,11 @@
     </row>
     <row r="513" spans="1:3" outlineLevel="1">
       <c r="A513" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B513" s="7"/>
       <c r="C513" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="514" spans="1:3" outlineLevel="2">
@@ -5903,39 +6039,39 @@
     </row>
     <row r="515" spans="1:3" outlineLevel="2">
       <c r="A515" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B515" s="13"/>
       <c r="C515" s="12" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="516" spans="1:3" outlineLevel="3">
       <c r="A516" s="8"/>
       <c r="B516" s="8"/>
       <c r="C516" s="9" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="517" spans="1:3" outlineLevel="3">
       <c r="A517" s="8"/>
       <c r="B517" s="8"/>
       <c r="C517" s="9" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="518" spans="1:3" outlineLevel="3">
       <c r="A518" s="8"/>
       <c r="B518" s="8"/>
       <c r="C518" s="9" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="519" spans="1:3" outlineLevel="3">
       <c r="A519" s="8"/>
       <c r="B519" s="8"/>
       <c r="C519" s="9" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="520" spans="1:3" outlineLevel="2">
@@ -5945,60 +6081,60 @@
     </row>
     <row r="521" spans="1:3" outlineLevel="2">
       <c r="A521" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B521" s="13"/>
       <c r="C521" s="12" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="522" spans="1:3" outlineLevel="3">
       <c r="A522" s="8"/>
       <c r="B522" s="8"/>
       <c r="C522" s="9" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="523" spans="1:3" outlineLevel="3">
       <c r="A523" s="8"/>
       <c r="B523" s="8"/>
       <c r="C523" s="9" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="524" spans="1:3" outlineLevel="3">
       <c r="A524" s="8"/>
       <c r="B524" s="8"/>
       <c r="C524" s="9" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="525" spans="1:3" outlineLevel="3">
       <c r="A525" s="8"/>
       <c r="B525" s="8"/>
       <c r="C525" s="9" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="526" spans="1:3" outlineLevel="3">
       <c r="A526" s="8"/>
       <c r="B526" s="8"/>
       <c r="C526" s="9" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="527" spans="1:3" outlineLevel="3">
       <c r="A527" s="8"/>
       <c r="B527" s="8"/>
       <c r="C527" s="9" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="528" spans="1:3" outlineLevel="3">
       <c r="A528" s="8"/>
       <c r="B528" s="8"/>
       <c r="C528" s="9" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="529" spans="1:3" outlineLevel="2">
@@ -6008,39 +6144,39 @@
     </row>
     <row r="530" spans="1:3" outlineLevel="2">
       <c r="A530" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B530" s="13"/>
       <c r="C530" s="12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="531" spans="1:3" outlineLevel="3">
       <c r="A531" s="8"/>
       <c r="B531" s="8"/>
       <c r="C531" s="9" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="532" spans="1:3" outlineLevel="3">
       <c r="A532" s="8"/>
       <c r="B532" s="8"/>
       <c r="C532" s="9" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="533" spans="1:3" outlineLevel="3">
       <c r="A533" s="8"/>
       <c r="B533" s="8"/>
       <c r="C533" s="9" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="534" spans="1:3" outlineLevel="3">
       <c r="A534" s="8"/>
       <c r="B534" s="8"/>
       <c r="C534" s="9" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="535" spans="1:3" outlineLevel="2">
@@ -6050,39 +6186,39 @@
     </row>
     <row r="536" spans="1:3" outlineLevel="2">
       <c r="A536" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B536" s="13"/>
       <c r="C536" s="12" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="537" spans="1:3" outlineLevel="3">
       <c r="A537" s="8"/>
       <c r="B537" s="8"/>
       <c r="C537" s="9" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="538" spans="1:3" outlineLevel="3">
       <c r="A538" s="8"/>
       <c r="B538" s="8"/>
       <c r="C538" s="9" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="539" spans="1:3" outlineLevel="3">
       <c r="A539" s="8"/>
       <c r="B539" s="8"/>
       <c r="C539" s="9" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="540" spans="1:3" outlineLevel="3">
       <c r="A540" s="8"/>
       <c r="B540" s="8"/>
       <c r="C540" s="9" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="541" spans="1:3" outlineLevel="2">
@@ -6092,39 +6228,39 @@
     </row>
     <row r="542" spans="1:3" outlineLevel="2">
       <c r="A542" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B542" s="13"/>
-      <c r="C542" s="17" t="s">
-        <v>551</v>
+      <c r="C542" s="13" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="543" spans="1:3" outlineLevel="3">
       <c r="A543" s="8"/>
       <c r="B543" s="8"/>
       <c r="C543" s="9" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="544" spans="1:3" outlineLevel="3">
       <c r="A544" s="8"/>
       <c r="B544" s="8"/>
       <c r="C544" s="9" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="545" spans="1:3" outlineLevel="3">
       <c r="A545" s="8"/>
       <c r="B545" s="8"/>
-      <c r="C545" s="16" t="s">
-        <v>554</v>
+      <c r="C545" s="9" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="546" spans="1:3" outlineLevel="3">
       <c r="A546" s="8"/>
       <c r="B546" s="8"/>
       <c r="C546" s="9" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="547" spans="1:3" outlineLevel="2">
@@ -6134,67 +6270,67 @@
     </row>
     <row r="548" spans="1:3" outlineLevel="2">
       <c r="A548" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B548" s="13"/>
       <c r="C548" s="12" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="549" spans="1:3" outlineLevel="3">
       <c r="A549" s="8"/>
       <c r="B549" s="8"/>
       <c r="C549" s="9" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
     </row>
     <row r="550" spans="1:3" outlineLevel="3">
       <c r="A550" s="8"/>
       <c r="B550" s="8"/>
       <c r="C550" s="9" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="551" spans="1:3" outlineLevel="3">
       <c r="A551" s="8"/>
       <c r="B551" s="8"/>
       <c r="C551" s="9" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="552" spans="1:3" outlineLevel="3">
       <c r="A552" s="8"/>
       <c r="B552" s="8"/>
       <c r="C552" s="9" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="553" spans="1:3" outlineLevel="3">
       <c r="A553" s="8"/>
       <c r="B553" s="8"/>
       <c r="C553" s="9" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="554" spans="1:3" outlineLevel="3">
       <c r="A554" s="8"/>
       <c r="B554" s="8"/>
       <c r="C554" s="9" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="555" spans="1:3" outlineLevel="3">
       <c r="A555" s="8"/>
       <c r="B555" s="8"/>
       <c r="C555" s="9" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="556" spans="1:3" outlineLevel="3">
       <c r="A556" s="8"/>
       <c r="B556" s="8"/>
       <c r="C556" s="9" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="557" spans="1:3" ht="16" thickBot="1">

</xml_diff>